<commit_message>
Add translations of the Website.resx to translations.html + use newlines beside <br/>
</commit_message>
<xml_diff>
--- a/docs/invariant/translations.xlsx
+++ b/docs/invariant/translations.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1671" uniqueCount="956">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1711" uniqueCount="976">
   <si>
     <t xml:space="preserve">Project</t>
   </si>
@@ -61,7 +61,7 @@
     <t xml:space="preserve">Learn8 your way ("Learn it your way") is a widely applicable study tool. Study languages, memorize names and faces, practice mental arithmetic, improve your math skills, rote learn topography or train your short term memory for any random subject.
 How does Learn8 work?
 - Create your own learn items - optionally with hints and feedback - or import items that other people have shared with you.
-- Start a (daily) learn flow for a set of items by selecting the tags that you do or do not want to study today.
+- Start a (daily) learning session for a set of items by selecting the tags that you do or do not want to study today.
 - Share your items with friends, colleagues or students easily via WhatsApp, Mail or via your website.
 - You can have multiple accounts on one device.
 - You can synchronize your learning progress between multiple devices.
@@ -80,7 +80,7 @@
     <t xml:space="preserve">Learn8 your way ("Learn it your way") is a widely applicable study tool. Study languages, memorise names and faces, practise mental arithmetics, improve your maths skills, rote learn topography or train your short term memory for any random subject.
 How does Learn8 work?
 - Create your own learn items - optionally with hints and feedback - or import items that other people have shared with you.
-- Start a (daily) learn flow for a set of items by selecting the tags that you do or do not want to study today.
+- Start a (daily) learning session for a set of items by selecting the tags that you do or do not want to study today.
 - Share your items with friends, colleagues or students easily via WhatsApp, Mail or via your website.
 - You can have multiple accounts on one device.
 - You can synchronise your learning progress between multiple devices.
@@ -762,7 +762,7 @@
 Other L8_KEYBOARD-options for mobile devices: EMAIL, TELEPHONE.
 The line
 L8_KEYBOARD = LATEX
-works on all devices. It uses the default keyboard, but the mathematical formulas that correspond to what you've just typed are shown instantly. When LaTeX-answers are checked during a learn flow, whitespace is ignored. This means for example that "x  +  1" is considered the same as "x+1".</t>
+works on all devices. It uses the default keyboard, but the mathematical formulas that correspond to what you've just typed are shown instantly. When LaTeX-answers are checked during a learning session, whitespace is ignored. This means for example that "x  +  1" is considered the same as "x+1".</t>
   </si>
   <si>
     <t xml:space="preserve">This resx file is not complete. It only contains the entries that require deviation form the default en-US:
@@ -1579,7 +1579,7 @@
     <t xml:space="preserve">ProgressIndicatorLabel_This_learn_flow</t>
   </si>
   <si>
-    <t xml:space="preserve">This learn flow</t>
+    <t xml:space="preserve">This learning session</t>
   </si>
   <si>
     <t xml:space="preserve">Deze leersessie</t>
@@ -1681,7 +1681,7 @@
     <t xml:space="preserve">Start_a_learn_flow</t>
   </si>
   <si>
-    <t xml:space="preserve">Start a learn flow</t>
+    <t xml:space="preserve">Start a learning session</t>
   </si>
   <si>
     <t xml:space="preserve">Start een leersessie</t>
@@ -1702,7 +1702,7 @@
     <t xml:space="preserve">Resume_learn_flow</t>
   </si>
   <si>
-    <t xml:space="preserve">Resume learn flow</t>
+    <t xml:space="preserve">Resume learning session</t>
   </si>
   <si>
     <t xml:space="preserve">Leersessie hervatten</t>
@@ -1711,7 +1711,7 @@
     <t xml:space="preserve">Start_a_new_learn_flow</t>
   </si>
   <si>
-    <t xml:space="preserve">Start a new learn flow</t>
+    <t xml:space="preserve">Start a new learning session</t>
   </si>
   <si>
     <t xml:space="preserve">Start een nieuwe leersessie</t>
@@ -2307,7 +2307,7 @@
     <t xml:space="preserve">Info_Goal_CorrectAnswersPerLearnFlow</t>
   </si>
   <si>
-    <t xml:space="preserve">The (daily) learn flow is completed when you have provided a certain number of correct answers during that learn flow.</t>
+    <t xml:space="preserve">The (daily) learning session is completed when you have provided a certain number of correct answers during that learning session.</t>
   </si>
   <si>
     <t xml:space="preserve">De (dagelijkse) leersessie is voltooid zodra je een bepaald (totaal) aantal correcte antwoorden hebt gegeven tijdens die leersessie.</t>
@@ -2316,7 +2316,7 @@
     <t xml:space="preserve">Info_LearnInGroupsOf</t>
   </si>
   <si>
-    <t xml:space="preserve">During a learn flow, new items are introduced to you in small groups. If too many items turn out to be hard, they are also presented in smaller groups. What size should such a group be?</t>
+    <t xml:space="preserve">During a learning session, new items are introduced to you in small groups. If too many items turn out to be hard, they are also presented in smaller groups. What size should such a group be?</t>
   </si>
   <si>
     <t xml:space="preserve">Tijdens een leersessie worden nieuwe items aan je voorgelegd in kleine groepjes. Ook als er te veel items moeilijk blijken te zijn, oefen je de items in kleine groepjes. Hoe groot mag zo'n groepje zijn?</t>
@@ -2325,11 +2325,11 @@
     <t xml:space="preserve">Info_NewOrUnfinishedItemsPerLearnFlow</t>
   </si>
   <si>
-    <t xml:space="preserve">A new learn flow will consist of
-- the hard* items of the previous learn flow
+    <t xml:space="preserve">A new learning session will consist of
+- the hard* items of the previous learning session
 - new items (if it fits)
 - mastered items for rehearsal
-How many new + hard items would you like to study per (daily) learn flow?
+How many new + hard items would you like to study per (daily) learning session?
 * An item is considered to be 'hard' if its score is 20% below the learning goal.</t>
   </si>
   <si>
@@ -2355,7 +2355,7 @@
     <t xml:space="preserve">Info_WarmingUpItems</t>
   </si>
   <si>
-    <t xml:space="preserve">Each learn flow starts with the rehearsal of items, without asking any item twice. How many items would you like to rehearse during this 'warming up'?</t>
+    <t xml:space="preserve">Each learning session starts with the rehearsal of items, without asking any item twice. How many items would you like to rehearse during this 'warming up'?</t>
   </si>
   <si>
     <t xml:space="preserve">Elke leersessie start met het herhalen van items, zonder enig item twee keer voor te leggen. Hoeveel items zou je voorgelegd willen krijgen tijdens deze 'warming up'?</t>
@@ -2442,15 +2442,6 @@
     <t xml:space="preserve">Synchroniseer nu</t>
   </si>
   <si>
-    <t xml:space="preserve">tbLocalSyncFolder_prefix</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Local sync folder:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lokale synchronisatiemap:</t>
-  </si>
-  <si>
     <t xml:space="preserve">The_symbols_you_would_like_to_consider_equal</t>
   </si>
   <si>
@@ -2490,7 +2481,7 @@
     <t xml:space="preserve">Validation_LearnInGroupsOf_Xmin_Xmax</t>
   </si>
   <si>
-    <t xml:space="preserve">Minimum is {0} and cannot be greater than ('new or unfinished items per learn flow') {1}.</t>
+    <t xml:space="preserve">Minimum is {0} and cannot be greater than ('new or unfinished items per learning session') {1}.</t>
   </si>
   <si>
     <t xml:space="preserve">Minimaal {0} en maximaal ('nieuwe of moeilijke items per leersessie') {1}.</t>
@@ -3047,7 +3038,7 @@
     <t xml:space="preserve">Over</t>
   </si>
   <si>
-    <t xml:space="preserve">App</t>
+    <t xml:space="preserve">Get_the_app</t>
   </si>
   <si>
     <t xml:space="preserve">Get the app</t>
@@ -3059,10 +3050,10 @@
     <t xml:space="preserve">AvailableFor</t>
   </si>
   <si>
-    <t xml:space="preserve">The app is currently only available for Windows 10 and Android. If you'd like this app to be available for iPhone too, let it know via the 'Development' section!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">De app is op dit moment alleen verkrijgbaar voor Windows 10 en Android. Als je deze app ook voor iPhone zou willen hebben, laat het weten via de 'Ontwikkeling' sectie!</t>
+    <t xml:space="preserve">The app is available for Windows 10 and Android. If you'd like this app to be available for iPhone too, let it know via the 'Development' section!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">De app is verkrijgbaar voor Windows 10 en Android. Als je deze app ook voor iPhone zou willen hebben, laat het weten via de 'Ontwikkeling' sectie!</t>
   </si>
   <si>
     <t xml:space="preserve">Coming_soon_</t>
@@ -3080,24 +3071,91 @@
     <t xml:space="preserve">Ontwikkeling</t>
   </si>
   <si>
-    <t xml:space="preserve">Development_Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Learn8 your way is still in development. If your would like to contribute, for example by translating the app to your language, please send a message to learn8yourway@gmail.com.
-Feedback and feature requests are welcome too!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Learn8 your way is nog in ontwikkeling. Als je een bijdrage zou willen leveren, bijvoorbeeld door de app te vertalen naar jouw taal, laat het weten via learn8yourway@gmail.com.
-Feedback en ideeën voor nieuwe functies zijn ook welkom!</t>
+    <t xml:space="preserve">Development_Introduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learn8 your way is still in development. There are several ways you can help!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learn8 your way is in ontwikkeling. Als je wil meehelpen, dan kan dat!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step1__Download_currently_available_translations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step 1: Download currently available translations. Choose one of the files:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stap 1: Download de vertalingen die op dit moment beschikbaar zijn. Kies een van de bestanden:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LanguageList_PageTitle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List of language codes for translators</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lijst met taalcodes voor vertalers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Language_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step2__Look_up_your_language_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step 2: Look up your language code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stap 2: Zoek jouw taalcode op</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please_send_an_e-mail_to_X_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please send an e-mail to {0}.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stuur een e-mail naar {0}.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Request_a_new_feature__report_a_bug_or_give_other_feedback</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Request a new feature, report a bug or give other feedback</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stel een uitbreiding voor (een "feature request"), meld een fout of geef andere feedback</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step3__Send_the_updated_file_to_X_or_upload_it_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step 3: Send the file with your modifications and/or additions to {0} or upload it.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stap 3: Verstuur het bestand met jouw aanpassingen en/of toevoegingen naar {0} of upload het.</t>
   </si>
   <si>
     <t xml:space="preserve">Share_items_that_you_have_created_or_download_items_that_others_have_shared_</t>
   </si>
   <si>
-    <t xml:space="preserve">Share items that you have created or download items that others have shared.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deel items die jij hebt gemaakt of download items die anderen hebben gedeeld.</t>
+    <t xml:space="preserve">Share Learn8 items that you have created or download items that others have shared.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deel Learn8 items die jij hebt gemaakt of download items die anderen hebben gedeeld.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Translate_the_app_to_another_language_or_correct_language_mistakes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Translate the app to your language or correct language mistakes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vertaal de app naar je eigen taal of corrigeer taalfouten</t>
   </si>
 </sst>
 </file>
@@ -3201,7 +3259,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I328"/>
+  <dimension ref="A1:I336"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
@@ -7757,7 +7815,7 @@
         <v>757</v>
       </c>
       <c r="I262" s="0" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7768,10 +7826,10 @@
         <v>642</v>
       </c>
       <c r="C263" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="E263" s="0" t="s">
         <v>759</v>
-      </c>
-      <c r="E263" s="0" t="s">
-        <v>760</v>
       </c>
       <c r="I263" s="0" t="s">
         <v>760</v>
@@ -7850,16 +7908,16 @@
         <v>8</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>642</v>
+        <v>773</v>
       </c>
       <c r="C268" s="1" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="E268" s="0" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="I268" s="0" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7867,7 +7925,7 @@
         <v>8</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="C269" s="1" t="s">
         <v>777</v>
@@ -7884,7 +7942,7 @@
         <v>8</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="C270" s="1" t="s">
         <v>780</v>
@@ -7901,7 +7959,7 @@
         <v>8</v>
       </c>
       <c r="B271" s="1" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="C271" s="1" t="s">
         <v>783</v>
@@ -7918,7 +7976,7 @@
         <v>8</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="C272" s="1" t="s">
         <v>786</v>
@@ -7935,7 +7993,7 @@
         <v>8</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="C273" s="1" t="s">
         <v>789</v>
@@ -7952,7 +8010,7 @@
         <v>8</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="C274" s="1" t="s">
         <v>792</v>
@@ -7969,7 +8027,7 @@
         <v>8</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="C275" s="1" t="s">
         <v>795</v>
@@ -7986,7 +8044,7 @@
         <v>8</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="C276" s="1" t="s">
         <v>798</v>
@@ -8003,7 +8061,7 @@
         <v>8</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="C277" s="1" t="s">
         <v>801</v>
@@ -8020,7 +8078,7 @@
         <v>8</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="C278" s="1" t="s">
         <v>804</v>
@@ -8037,7 +8095,7 @@
         <v>8</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="C279" s="1" t="s">
         <v>807</v>
@@ -8054,7 +8112,7 @@
         <v>8</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="C280" s="1" t="s">
         <v>810</v>
@@ -8071,7 +8129,7 @@
         <v>8</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="C281" s="1" t="s">
         <v>813</v>
@@ -8088,7 +8146,7 @@
         <v>8</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="C282" s="1" t="s">
         <v>816</v>
@@ -8105,7 +8163,7 @@
         <v>8</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="C283" s="1" t="s">
         <v>819</v>
@@ -8122,7 +8180,7 @@
         <v>8</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="C284" s="1" t="s">
         <v>822</v>
@@ -8139,7 +8197,7 @@
         <v>8</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="C285" s="1" t="s">
         <v>825</v>
@@ -8156,7 +8214,7 @@
         <v>8</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="C286" s="1" t="s">
         <v>828</v>
@@ -8173,7 +8231,7 @@
         <v>8</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="C287" s="1" t="s">
         <v>831</v>
@@ -8190,7 +8248,7 @@
         <v>8</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="C288" s="1" t="s">
         <v>834</v>
@@ -8207,7 +8265,7 @@
         <v>8</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="C289" s="1" t="s">
         <v>837</v>
@@ -8224,7 +8282,7 @@
         <v>8</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="C290" s="1" t="s">
         <v>840</v>
@@ -8241,16 +8299,16 @@
         <v>8</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>776</v>
+        <v>843</v>
       </c>
       <c r="C291" s="1" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="E291" s="0" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="I291" s="0" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8258,7 +8316,7 @@
         <v>8</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C292" s="1" t="s">
         <v>847</v>
@@ -8275,16 +8333,16 @@
         <v>8</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C293" s="1" t="s">
         <v>850</v>
       </c>
       <c r="E293" s="0" t="s">
+        <v>850</v>
+      </c>
+      <c r="I293" s="0" t="s">
         <v>851</v>
-      </c>
-      <c r="I293" s="0" t="s">
-        <v>852</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8292,10 +8350,10 @@
         <v>8</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C294" s="1" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="E294" s="0" t="s">
         <v>853</v>
@@ -8309,7 +8367,7 @@
         <v>8</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C295" s="1" t="s">
         <v>855</v>
@@ -8326,7 +8384,7 @@
         <v>8</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C296" s="1" t="s">
         <v>858</v>
@@ -8343,7 +8401,7 @@
         <v>8</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C297" s="1" t="s">
         <v>861</v>
@@ -8360,7 +8418,7 @@
         <v>8</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C298" s="1" t="s">
         <v>864</v>
@@ -8377,7 +8435,7 @@
         <v>8</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C299" s="1" t="s">
         <v>867</v>
@@ -8394,7 +8452,7 @@
         <v>8</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C300" s="1" t="s">
         <v>870</v>
@@ -8411,7 +8469,7 @@
         <v>8</v>
       </c>
       <c r="B301" s="1" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C301" s="1" t="s">
         <v>873</v>
@@ -8428,7 +8486,7 @@
         <v>8</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C302" s="1" t="s">
         <v>876</v>
@@ -8440,37 +8498,37 @@
         <v>878</v>
       </c>
     </row>
-    <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="303" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B303" s="1" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C303" s="1" t="s">
         <v>879</v>
       </c>
-      <c r="E303" s="0" t="s">
+      <c r="E303" s="2" t="s">
         <v>880</v>
       </c>
-      <c r="I303" s="0" t="s">
+      <c r="I303" s="2" t="s">
         <v>881</v>
       </c>
     </row>
-    <row r="304" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C304" s="1" t="s">
         <v>882</v>
       </c>
-      <c r="E304" s="2" t="s">
+      <c r="E304" s="0" t="s">
         <v>883</v>
       </c>
-      <c r="I304" s="2" t="s">
+      <c r="I304" s="0" t="s">
         <v>884</v>
       </c>
     </row>
@@ -8479,7 +8537,7 @@
         <v>8</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C305" s="1" t="s">
         <v>885</v>
@@ -8496,7 +8554,7 @@
         <v>8</v>
       </c>
       <c r="B306" s="1" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C306" s="1" t="s">
         <v>888</v>
@@ -8505,7 +8563,7 @@
         <v>889</v>
       </c>
       <c r="I306" s="0" t="s">
-        <v>890</v>
+        <v>887</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8513,16 +8571,16 @@
         <v>8</v>
       </c>
       <c r="B307" s="1" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C307" s="1" t="s">
+        <v>890</v>
+      </c>
+      <c r="E307" s="0" t="s">
         <v>891</v>
       </c>
-      <c r="E307" s="0" t="s">
+      <c r="I307" s="0" t="s">
         <v>892</v>
-      </c>
-      <c r="I307" s="0" t="s">
-        <v>890</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8530,7 +8588,7 @@
         <v>8</v>
       </c>
       <c r="B308" s="1" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C308" s="1" t="s">
         <v>893</v>
@@ -8547,7 +8605,7 @@
         <v>8</v>
       </c>
       <c r="B309" s="1" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C309" s="1" t="s">
         <v>896</v>
@@ -8564,7 +8622,7 @@
         <v>8</v>
       </c>
       <c r="B310" s="1" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C310" s="1" t="s">
         <v>899</v>
@@ -8581,7 +8639,7 @@
         <v>8</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C311" s="1" t="s">
         <v>902</v>
@@ -8598,7 +8656,7 @@
         <v>8</v>
       </c>
       <c r="B312" s="1" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C312" s="1" t="s">
         <v>905</v>
@@ -8615,7 +8673,7 @@
         <v>8</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C313" s="1" t="s">
         <v>908</v>
@@ -8632,7 +8690,7 @@
         <v>8</v>
       </c>
       <c r="B314" s="1" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C314" s="1" t="s">
         <v>911</v>
@@ -8649,7 +8707,7 @@
         <v>8</v>
       </c>
       <c r="B315" s="1" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C315" s="1" t="s">
         <v>914</v>
@@ -8666,7 +8724,7 @@
         <v>8</v>
       </c>
       <c r="B316" s="1" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C316" s="1" t="s">
         <v>917</v>
@@ -8683,7 +8741,7 @@
         <v>8</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C317" s="1" t="s">
         <v>920</v>
@@ -8700,7 +8758,7 @@
         <v>8</v>
       </c>
       <c r="B318" s="1" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C318" s="1" t="s">
         <v>923</v>
@@ -8717,7 +8775,7 @@
         <v>8</v>
       </c>
       <c r="B319" s="1" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C319" s="1" t="s">
         <v>926</v>
@@ -8734,7 +8792,7 @@
         <v>8</v>
       </c>
       <c r="B320" s="1" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C320" s="1" t="s">
         <v>929</v>
@@ -8748,30 +8806,30 @@
     </row>
     <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="1" t="s">
-        <v>8</v>
+        <v>932</v>
       </c>
       <c r="B321" s="1" t="s">
-        <v>846</v>
+        <v>933</v>
       </c>
       <c r="C321" s="1" t="s">
-        <v>932</v>
+        <v>934</v>
       </c>
       <c r="E321" s="0" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="I321" s="0" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="1" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
       <c r="B322" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="C322" s="1" t="s">
         <v>936</v>
-      </c>
-      <c r="C322" s="1" t="s">
-        <v>937</v>
       </c>
       <c r="E322" s="0" t="s">
         <v>937</v>
@@ -8782,10 +8840,10 @@
     </row>
     <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="1" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>936</v>
+        <v>933</v>
       </c>
       <c r="C323" s="1" t="s">
         <v>939</v>
@@ -8799,10 +8857,10 @@
     </row>
     <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="1" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
       <c r="B324" s="1" t="s">
-        <v>936</v>
+        <v>933</v>
       </c>
       <c r="C324" s="1" t="s">
         <v>942</v>
@@ -8816,30 +8874,30 @@
     </row>
     <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="1" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
       <c r="B325" s="1" t="s">
-        <v>936</v>
+        <v>933</v>
       </c>
       <c r="C325" s="1" t="s">
         <v>945</v>
       </c>
       <c r="E325" s="0" t="s">
+        <v>945</v>
+      </c>
+      <c r="I325" s="0" t="s">
         <v>946</v>
-      </c>
-      <c r="I325" s="0" t="s">
-        <v>947</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="1" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
       <c r="B326" s="1" t="s">
-        <v>936</v>
+        <v>933</v>
       </c>
       <c r="C326" s="1" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="E326" s="0" t="s">
         <v>948</v>
@@ -8848,38 +8906,174 @@
         <v>949</v>
       </c>
     </row>
-    <row r="327" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="1" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
       <c r="B327" s="1" t="s">
-        <v>936</v>
+        <v>933</v>
       </c>
       <c r="C327" s="1" t="s">
         <v>950</v>
       </c>
-      <c r="E327" s="2" t="s">
+      <c r="E327" s="0" t="s">
         <v>951</v>
       </c>
-      <c r="I327" s="2" t="s">
+      <c r="I327" s="0" t="s">
         <v>952</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="1" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
       <c r="B328" s="1" t="s">
-        <v>936</v>
+        <v>933</v>
       </c>
       <c r="C328" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E328" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="I328" s="0" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A329" s="1" t="s">
+        <v>932</v>
+      </c>
+      <c r="B329" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="C329" s="1" t="s">
         <v>953</v>
       </c>
-      <c r="E328" s="0" t="s">
+      <c r="E329" s="0" t="s">
         <v>954</v>
       </c>
-      <c r="I328" s="0" t="s">
+      <c r="I329" s="0" t="s">
         <v>955</v>
+      </c>
+    </row>
+    <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A330" s="1" t="s">
+        <v>932</v>
+      </c>
+      <c r="B330" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="C330" s="1" t="s">
+        <v>956</v>
+      </c>
+      <c r="E330" s="0" t="s">
+        <v>957</v>
+      </c>
+      <c r="I330" s="0" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A331" s="1" t="s">
+        <v>932</v>
+      </c>
+      <c r="B331" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="C331" s="1" t="s">
+        <v>958</v>
+      </c>
+      <c r="E331" s="0" t="s">
+        <v>959</v>
+      </c>
+      <c r="I331" s="0" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A332" s="1" t="s">
+        <v>932</v>
+      </c>
+      <c r="B332" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="C332" s="1" t="s">
+        <v>961</v>
+      </c>
+      <c r="E332" s="0" t="s">
+        <v>962</v>
+      </c>
+      <c r="I332" s="0" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A333" s="1" t="s">
+        <v>932</v>
+      </c>
+      <c r="B333" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="C333" s="1" t="s">
+        <v>964</v>
+      </c>
+      <c r="E333" s="0" t="s">
+        <v>965</v>
+      </c>
+      <c r="I333" s="0" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A334" s="1" t="s">
+        <v>932</v>
+      </c>
+      <c r="B334" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="C334" s="1" t="s">
+        <v>967</v>
+      </c>
+      <c r="E334" s="0" t="s">
+        <v>968</v>
+      </c>
+      <c r="I334" s="0" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A335" s="1" t="s">
+        <v>932</v>
+      </c>
+      <c r="B335" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="C335" s="1" t="s">
+        <v>970</v>
+      </c>
+      <c r="E335" s="0" t="s">
+        <v>971</v>
+      </c>
+      <c r="I335" s="0" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A336" s="1" t="s">
+        <v>932</v>
+      </c>
+      <c r="B336" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="C336" s="1" t="s">
+        <v>973</v>
+      </c>
+      <c r="E336" s="0" t="s">
+        <v>974</v>
+      </c>
+      <c r="I336" s="0" t="s">
+        <v>975</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Contact form: Google Form with Formfacade
</commit_message>
<xml_diff>
--- a/docs/invariant/translations.xlsx
+++ b/docs/invariant/translations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1711" uniqueCount="976">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1721" uniqueCount="982">
   <si>
     <t xml:space="preserve">Project</t>
   </si>
@@ -3113,15 +3113,6 @@
     <t xml:space="preserve">Stap 2: Zoek jouw taalcode op</t>
   </si>
   <si>
-    <t xml:space="preserve">Please_send_an_e-mail_to_X_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please send an e-mail to {0}.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stuur een e-mail naar {0}.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Request_a_new_feature__report_a_bug_or_give_other_feedback</t>
   </si>
   <si>
@@ -3131,15 +3122,6 @@
     <t xml:space="preserve">Stel een uitbreiding voor (een "feature request"), meld een fout of geef andere feedback</t>
   </si>
   <si>
-    <t xml:space="preserve">Step3__Send_the_updated_file_to_X_or_upload_it_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Step 3: Send the file with your modifications and/or additions to {0} or upload it.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stap 3: Verstuur het bestand met jouw aanpassingen en/of toevoegingen naar {0} of upload het.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Share_items_that_you_have_created_or_download_items_that_others_have_shared_</t>
   </si>
   <si>
@@ -3156,6 +3138,42 @@
   </si>
   <si>
     <t xml:space="preserve">Vertaal de app naar je eigen taal of corrigeer taalfouten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step3__Send_the_updated_file_to_X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step 3: Send the file with your modifications and/or additions to {0}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stap 3: Verstuur het bestand met jouw aanpassingen en/of toevoegingen naar {0}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact_form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contactformulier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">use_the_contact_form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">use the contact form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gebruik het contactformulier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Send_an_e-mail_to_X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Send an e-mail to {0}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stuur een e-mail naar {0}</t>
   </si>
 </sst>
 </file>
@@ -3170,6 +3188,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -3259,7 +3278,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I336"/>
+  <dimension ref="A1:I338"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
@@ -9076,6 +9095,40 @@
         <v>975</v>
       </c>
     </row>
+    <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A337" s="1" t="s">
+        <v>932</v>
+      </c>
+      <c r="B337" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="C337" s="1" t="s">
+        <v>976</v>
+      </c>
+      <c r="E337" s="0" t="s">
+        <v>977</v>
+      </c>
+      <c r="I337" s="0" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A338" s="1" t="s">
+        <v>932</v>
+      </c>
+      <c r="B338" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="C338" s="1" t="s">
+        <v>979</v>
+      </c>
+      <c r="E338" s="0" t="s">
+        <v>980</v>
+      </c>
+      <c r="I338" s="0" t="s">
+        <v>981</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Revert "Add Contact form: Google Form with Formfacade"
This reverts commit f0ad614f96bf0fbabcf8be1e768955a1e588da49.
</commit_message>
<xml_diff>
--- a/docs/invariant/translations.xlsx
+++ b/docs/invariant/translations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1721" uniqueCount="982">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1711" uniqueCount="976">
   <si>
     <t xml:space="preserve">Project</t>
   </si>
@@ -3113,6 +3113,15 @@
     <t xml:space="preserve">Stap 2: Zoek jouw taalcode op</t>
   </si>
   <si>
+    <t xml:space="preserve">Please_send_an_e-mail_to_X_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please send an e-mail to {0}.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stuur een e-mail naar {0}.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Request_a_new_feature__report_a_bug_or_give_other_feedback</t>
   </si>
   <si>
@@ -3122,6 +3131,15 @@
     <t xml:space="preserve">Stel een uitbreiding voor (een "feature request"), meld een fout of geef andere feedback</t>
   </si>
   <si>
+    <t xml:space="preserve">Step3__Send_the_updated_file_to_X_or_upload_it_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step 3: Send the file with your modifications and/or additions to {0} or upload it.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stap 3: Verstuur het bestand met jouw aanpassingen en/of toevoegingen naar {0} of upload het.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Share_items_that_you_have_created_or_download_items_that_others_have_shared_</t>
   </si>
   <si>
@@ -3138,42 +3156,6 @@
   </si>
   <si>
     <t xml:space="preserve">Vertaal de app naar je eigen taal of corrigeer taalfouten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Step3__Send_the_updated_file_to_X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Step 3: Send the file with your modifications and/or additions to {0}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stap 3: Verstuur het bestand met jouw aanpassingen en/of toevoegingen naar {0}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact_form</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact form</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contactformulier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">use_the_contact_form</t>
-  </si>
-  <si>
-    <t xml:space="preserve">use the contact form</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gebruik het contactformulier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Send_an_e-mail_to_X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Send an e-mail to {0}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stuur een e-mail naar {0}</t>
   </si>
 </sst>
 </file>
@@ -3188,7 +3170,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -3278,7 +3259,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I338"/>
+  <dimension ref="A1:I336"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
@@ -9095,40 +9076,6 @@
         <v>975</v>
       </c>
     </row>
-    <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A337" s="1" t="s">
-        <v>932</v>
-      </c>
-      <c r="B337" s="1" t="s">
-        <v>933</v>
-      </c>
-      <c r="C337" s="1" t="s">
-        <v>976</v>
-      </c>
-      <c r="E337" s="0" t="s">
-        <v>977</v>
-      </c>
-      <c r="I337" s="0" t="s">
-        <v>978</v>
-      </c>
-    </row>
-    <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A338" s="1" t="s">
-        <v>932</v>
-      </c>
-      <c r="B338" s="1" t="s">
-        <v>933</v>
-      </c>
-      <c r="C338" s="1" t="s">
-        <v>979</v>
-      </c>
-      <c r="E338" s="0" t="s">
-        <v>980</v>
-      </c>
-      <c r="I338" s="0" t="s">
-        <v>981</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Contact: use Google Form with FormFacade - vesion 2
</commit_message>
<xml_diff>
--- a/docs/invariant/translations.xlsx
+++ b/docs/invariant/translations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1711" uniqueCount="976">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1730" uniqueCount="985">
   <si>
     <t xml:space="preserve">Project</t>
   </si>
@@ -3113,13 +3113,13 @@
     <t xml:space="preserve">Stap 2: Zoek jouw taalcode op</t>
   </si>
   <si>
-    <t xml:space="preserve">Please_send_an_e-mail_to_X_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please send an e-mail to {0}.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stuur een e-mail naar {0}.</t>
+    <t xml:space="preserve">Send_an_e-mail_to_X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Send an e-mail to {0}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stuur een e-mail naar {0}</t>
   </si>
   <si>
     <t xml:space="preserve">Request_a_new_feature__report_a_bug_or_give_other_feedback</t>
@@ -3131,13 +3131,13 @@
     <t xml:space="preserve">Stel een uitbreiding voor (een "feature request"), meld een fout of geef andere feedback</t>
   </si>
   <si>
-    <t xml:space="preserve">Step3__Send_the_updated_file_to_X_or_upload_it_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Step 3: Send the file with your modifications and/or additions to {0} or upload it.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stap 3: Verstuur het bestand met jouw aanpassingen en/of toevoegingen naar {0} of upload het.</t>
+    <t xml:space="preserve">Step3__Send_the_updated_file_to_X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step 3: Send the file with your modifications and/or additions to {0}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stap 3: Verstuur het bestand met jouw aanpassingen en/of toevoegingen naar {0}</t>
   </si>
   <si>
     <t xml:space="preserve">Share_items_that_you_have_created_or_download_items_that_others_have_shared_</t>
@@ -3156,6 +3156,33 @@
   </si>
   <si>
     <t xml:space="preserve">Vertaal de app naar je eigen taal of corrigeer taalfouten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">use_the_contact_form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">use the contact form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gebruik het contactformulier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact_form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contactformulier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refresh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verversen</t>
   </si>
 </sst>
 </file>
@@ -3170,6 +3197,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -3259,7 +3287,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I336"/>
+  <dimension ref="A1:I340"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
@@ -9076,6 +9104,71 @@
         <v>975</v>
       </c>
     </row>
+    <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A337" s="1" t="s">
+        <v>932</v>
+      </c>
+      <c r="B337" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="C337" s="1" t="s">
+        <v>976</v>
+      </c>
+      <c r="E337" s="0" t="s">
+        <v>977</v>
+      </c>
+      <c r="I337" s="0" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A338" s="1" t="s">
+        <v>932</v>
+      </c>
+      <c r="B338" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="C338" s="1" t="s">
+        <v>979</v>
+      </c>
+      <c r="E338" s="0" t="s">
+        <v>980</v>
+      </c>
+      <c r="I338" s="0" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A339" s="1" t="s">
+        <v>932</v>
+      </c>
+      <c r="B339" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="C339" s="1" t="s">
+        <v>982</v>
+      </c>
+      <c r="E339" s="0" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A340" s="1" t="s">
+        <v>932</v>
+      </c>
+      <c r="B340" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="C340" s="1" t="s">
+        <v>983</v>
+      </c>
+      <c r="E340" s="0" t="s">
+        <v>983</v>
+      </c>
+      <c r="I340" s="0" t="s">
+        <v>984</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Add sharing information + update translations downloads
</commit_message>
<xml_diff>
--- a/docs/invariant/translations.xlsx
+++ b/docs/invariant/translations.xlsx
@@ -1871,29 +1871,6 @@
     <t xml:space="preserve">Item verwijderd.</t>
   </si>
   <si>
-    <t xml:space="preserve">JavaScriptConfirmationExplanation_XacceptAll_XtheScript_XdoNotAccept</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Learn8 items can use JavaScript (this is a programming language). This makes it possible to create an item that generates a different question each time it's asked (for example, for arithmetic or math).
-However, if you do not understand the JavaScript that is used, you should probably not import items that use it.
-An exception to this rule in case of students: if you received this share package directly from your school teacher, you might probably just choose '{0}'.
-One item uses the following JavaScript and you can answer whether you accept it not:
-====== The JavaScript starts here ======
-{1}
-======== ... and ends here ======== 
-If you click '{2}', the item will not be imported.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Learn8 items kunnen JavaScript gebruiken (dat is een programmeertaal). Daardoor wordt het mogelijk om items te maken dat telkens een nieuwe vraag genereert (bijvoorbeeld voor rekenen of wiskunde).
-Items die JavaScript gebruiken kan je misschien beter niet importeren als je de JavaScript ervan niet begrijpt.
-Een uitzondering op deze regel in het geval van leerlingen: als je dit gedeelde Learn8-bestand direct van je leraar hebt gekregen, dan kun je waarschijnlijk gewoon kiezen voor '{0}'.
-Een item gebruikt de volgende JavaScript en jij kan bepalen of je het accepteert of niet:
-====== De JavaScript begint hier ======
-{1}
-======== ... en eindigt hier ========
-Als je op '{2}' klikt, dan zal het item niet geïmporteerd worden.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Learn8_does_not_have_permission_to_read_the_file</t>
   </si>
   <si>
@@ -1937,15 +1914,6 @@
   </si>
   <si>
     <t xml:space="preserve">Geen samenvatting beschikbaar.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Only_accept_it_if_you_understand_it</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Only accept it if you understand it!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alleen accepteren als je het begrijpt!</t>
   </si>
   <si>
     <t xml:space="preserve">Please_dont_close_the_app</t>
@@ -3192,13 +3160,31 @@
     <t xml:space="preserve">Verversen</t>
   </si>
   <si>
-    <t xml:space="preserve">Shared_with_you</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shared with you</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gedeeld met jou</t>
+    <t xml:space="preserve">Shared_in_the_current_website_language</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shared in the current website language</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gedeeld in de huidige websitetaal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sharing_a_package_or_other_website</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Share a Learn8 package or share a link to another website</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Een Learn8 pakketje of een link naar een andere website delen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sharing_Info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You may have created a package that is useful for others or you know about another website for sharing learn8 files. Nice!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Je hebt misschien een pakketje gemaakt dat handig is voor anderen of je kent een website waar Learn8 pakketjes worden gedeeld. Gaaf!</t>
   </si>
 </sst>
 </file>
@@ -6812,7 +6798,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="203" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="1" t="s">
         <v>8</v>
       </c>
@@ -6822,10 +6808,10 @@
       <c r="C203" s="1" t="s">
         <v>569</v>
       </c>
-      <c r="E203" s="2" t="s">
+      <c r="E203" s="0" t="s">
         <v>570</v>
       </c>
-      <c r="I203" s="2" t="s">
+      <c r="I203" s="0" t="s">
         <v>571</v>
       </c>
     </row>
@@ -6956,13 +6942,13 @@
         <v>514</v>
       </c>
       <c r="C211" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E211" s="0" t="s">
         <v>593</v>
       </c>
-      <c r="E211" s="0" t="s">
+      <c r="I211" s="0" t="s">
         <v>594</v>
-      </c>
-      <c r="I211" s="0" t="s">
-        <v>595</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6973,13 +6959,13 @@
         <v>514</v>
       </c>
       <c r="C212" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="E212" s="0" t="s">
+        <v>595</v>
+      </c>
+      <c r="I212" s="0" t="s">
         <v>596</v>
-      </c>
-      <c r="E212" s="0" t="s">
-        <v>597</v>
-      </c>
-      <c r="I212" s="0" t="s">
-        <v>598</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6990,13 +6976,13 @@
         <v>514</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>101</v>
+        <v>597</v>
       </c>
       <c r="E213" s="0" t="s">
+        <v>598</v>
+      </c>
+      <c r="I213" s="0" t="s">
         <v>599</v>
-      </c>
-      <c r="I213" s="0" t="s">
-        <v>600</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7007,7 +6993,7 @@
         <v>514</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="E214" s="0" t="s">
         <v>601</v>
@@ -7084,7 +7070,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="219" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="1" t="s">
         <v>8</v>
       </c>
@@ -7094,10 +7080,10 @@
       <c r="C219" s="1" t="s">
         <v>615</v>
       </c>
-      <c r="E219" s="0" t="s">
+      <c r="E219" s="2" t="s">
         <v>616</v>
       </c>
-      <c r="I219" s="0" t="s">
+      <c r="I219" s="2" t="s">
         <v>617</v>
       </c>
     </row>
@@ -7118,7 +7104,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="221" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="1" t="s">
         <v>8</v>
       </c>
@@ -7128,10 +7114,10 @@
       <c r="C221" s="1" t="s">
         <v>621</v>
       </c>
-      <c r="E221" s="2" t="s">
+      <c r="E221" s="0" t="s">
         <v>622</v>
       </c>
-      <c r="I221" s="2" t="s">
+      <c r="I221" s="0" t="s">
         <v>623</v>
       </c>
     </row>
@@ -7233,8 +7219,11 @@
       <c r="E227" s="0" t="s">
         <v>640</v>
       </c>
+      <c r="G227" s="0" t="s">
+        <v>641</v>
+      </c>
       <c r="I227" s="0" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7242,16 +7231,16 @@
         <v>8</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>514</v>
+        <v>643</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="E228" s="0" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="I228" s="0" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7259,19 +7248,16 @@
         <v>8</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>514</v>
+        <v>643</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="E229" s="0" t="s">
-        <v>646</v>
-      </c>
-      <c r="G229" s="0" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="I229" s="0" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7279,7 +7265,7 @@
         <v>8</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C230" s="1" t="s">
         <v>650</v>
@@ -7296,7 +7282,7 @@
         <v>8</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C231" s="1" t="s">
         <v>653</v>
@@ -7313,7 +7299,7 @@
         <v>8</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C232" s="1" t="s">
         <v>656</v>
@@ -7330,7 +7316,7 @@
         <v>8</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C233" s="1" t="s">
         <v>659</v>
@@ -7338,8 +7324,14 @@
       <c r="E233" s="0" t="s">
         <v>660</v>
       </c>
+      <c r="F233" s="0" t="s">
+        <v>661</v>
+      </c>
+      <c r="G233" s="0" t="s">
+        <v>662</v>
+      </c>
       <c r="I233" s="0" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7347,16 +7339,22 @@
         <v>8</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="E234" s="0" t="s">
-        <v>663</v>
+        <v>664</v>
+      </c>
+      <c r="F234" s="0" t="s">
+        <v>665</v>
+      </c>
+      <c r="G234" s="0" t="s">
+        <v>666</v>
       </c>
       <c r="I234" s="0" t="s">
-        <v>664</v>
+        <v>667</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7364,22 +7362,16 @@
         <v>8</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>665</v>
+        <v>668</v>
       </c>
       <c r="E235" s="0" t="s">
-        <v>666</v>
-      </c>
-      <c r="F235" s="0" t="s">
-        <v>667</v>
-      </c>
-      <c r="G235" s="0" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="I235" s="0" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7387,22 +7379,22 @@
         <v>8</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="E236" s="0" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="F236" s="0" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c r="G236" s="0" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="I236" s="0" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7410,16 +7402,16 @@
         <v>8</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="E237" s="0" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
       <c r="I237" s="0" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7427,18 +7419,12 @@
         <v>8</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="E238" s="0" t="s">
-        <v>678</v>
-      </c>
-      <c r="F238" s="0" t="s">
-        <v>679</v>
-      </c>
-      <c r="G238" s="0" t="s">
         <v>680</v>
       </c>
       <c r="I238" s="0" t="s">
@@ -7450,7 +7436,7 @@
         <v>8</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C239" s="1" t="s">
         <v>682</v>
@@ -7458,8 +7444,14 @@
       <c r="E239" s="0" t="s">
         <v>683</v>
       </c>
+      <c r="F239" s="0" t="s">
+        <v>684</v>
+      </c>
+      <c r="G239" s="0" t="s">
+        <v>685</v>
+      </c>
       <c r="I239" s="0" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7467,16 +7459,19 @@
         <v>8</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="E240" s="0" t="s">
-        <v>686</v>
+        <v>688</v>
+      </c>
+      <c r="G240" s="0" t="s">
+        <v>689</v>
       </c>
       <c r="I240" s="0" t="s">
-        <v>687</v>
+        <v>690</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7484,41 +7479,32 @@
         <v>8</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C241" s="1" t="s">
-        <v>688</v>
+        <v>691</v>
       </c>
       <c r="E241" s="0" t="s">
-        <v>689</v>
-      </c>
-      <c r="F241" s="0" t="s">
-        <v>690</v>
-      </c>
-      <c r="G241" s="0" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="I241" s="0" t="s">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="242" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C242" s="1" t="s">
-        <v>693</v>
-      </c>
-      <c r="E242" s="0" t="s">
         <v>694</v>
       </c>
-      <c r="G242" s="0" t="s">
+      <c r="E242" s="2" t="s">
         <v>695</v>
       </c>
-      <c r="I242" s="0" t="s">
+      <c r="I242" s="2" t="s">
         <v>696</v>
       </c>
     </row>
@@ -7527,7 +7513,7 @@
         <v>8</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C243" s="1" t="s">
         <v>697</v>
@@ -7539,88 +7525,88 @@
         <v>699</v>
       </c>
     </row>
-    <row r="244" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C244" s="1" t="s">
         <v>700</v>
       </c>
-      <c r="E244" s="2" t="s">
+      <c r="E244" s="0" t="s">
         <v>701</v>
       </c>
-      <c r="I244" s="2" t="s">
+      <c r="I244" s="0" t="s">
         <v>702</v>
       </c>
     </row>
-    <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="245" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C245" s="1" t="s">
         <v>703</v>
       </c>
-      <c r="E245" s="0" t="s">
+      <c r="E245" s="2" t="s">
         <v>704</v>
       </c>
-      <c r="I245" s="0" t="s">
+      <c r="I245" s="2" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="246" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C246" s="1" t="s">
         <v>706</v>
       </c>
-      <c r="E246" s="0" t="s">
+      <c r="E246" s="2" t="s">
         <v>707</v>
       </c>
-      <c r="I246" s="0" t="s">
+      <c r="I246" s="2" t="s">
         <v>708</v>
       </c>
     </row>
-    <row r="247" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C247" s="1" t="s">
         <v>709</v>
       </c>
-      <c r="E247" s="2" t="s">
+      <c r="E247" s="0" t="s">
         <v>710</v>
       </c>
-      <c r="I247" s="2" t="s">
+      <c r="I247" s="0" t="s">
         <v>711</v>
       </c>
     </row>
-    <row r="248" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C248" s="1" t="s">
         <v>712</v>
       </c>
-      <c r="E248" s="2" t="s">
+      <c r="E248" s="0" t="s">
         <v>713</v>
       </c>
-      <c r="I248" s="2" t="s">
+      <c r="I248" s="0" t="s">
         <v>714</v>
       </c>
     </row>
@@ -7629,7 +7615,7 @@
         <v>8</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C249" s="1" t="s">
         <v>715</v>
@@ -7646,7 +7632,7 @@
         <v>8</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C250" s="1" t="s">
         <v>718</v>
@@ -7663,7 +7649,7 @@
         <v>8</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C251" s="1" t="s">
         <v>721</v>
@@ -7680,7 +7666,7 @@
         <v>8</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C252" s="1" t="s">
         <v>724</v>
@@ -7697,7 +7683,7 @@
         <v>8</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C253" s="1" t="s">
         <v>727</v>
@@ -7714,7 +7700,7 @@
         <v>8</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C254" s="1" t="s">
         <v>730</v>
@@ -7731,7 +7717,7 @@
         <v>8</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C255" s="1" t="s">
         <v>733</v>
@@ -7748,7 +7734,7 @@
         <v>8</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C256" s="1" t="s">
         <v>736</v>
@@ -7765,7 +7751,7 @@
         <v>8</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C257" s="1" t="s">
         <v>739</v>
@@ -7782,7 +7768,7 @@
         <v>8</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C258" s="1" t="s">
         <v>742</v>
@@ -7799,7 +7785,7 @@
         <v>8</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C259" s="1" t="s">
         <v>745</v>
@@ -7816,7 +7802,7 @@
         <v>8</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C260" s="1" t="s">
         <v>748</v>
@@ -7833,7 +7819,7 @@
         <v>8</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C261" s="1" t="s">
         <v>751</v>
@@ -7850,7 +7836,7 @@
         <v>8</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C262" s="1" t="s">
         <v>754</v>
@@ -7867,7 +7853,7 @@
         <v>8</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C263" s="1" t="s">
         <v>757</v>
@@ -7876,7 +7862,7 @@
         <v>758</v>
       </c>
       <c r="I263" s="0" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7884,16 +7870,16 @@
         <v>8</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C264" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="E264" s="0" t="s">
         <v>760</v>
       </c>
-      <c r="E264" s="0" t="s">
+      <c r="I264" s="0" t="s">
         <v>761</v>
-      </c>
-      <c r="I264" s="0" t="s">
-        <v>762</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7901,13 +7887,13 @@
         <v>8</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C265" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="E265" s="0" t="s">
         <v>763</v>
-      </c>
-      <c r="E265" s="0" t="s">
-        <v>764</v>
       </c>
       <c r="I265" s="0" t="s">
         <v>764</v>
@@ -7918,7 +7904,7 @@
         <v>8</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C266" s="1" t="s">
         <v>765</v>
@@ -7935,7 +7921,7 @@
         <v>8</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C267" s="1" t="s">
         <v>768</v>
@@ -7952,7 +7938,7 @@
         <v>8</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C268" s="1" t="s">
         <v>771</v>
@@ -7969,16 +7955,16 @@
         <v>8</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C269" s="1" t="s">
-        <v>774</v>
+        <v>153</v>
       </c>
       <c r="E269" s="0" t="s">
-        <v>775</v>
+        <v>153</v>
       </c>
       <c r="I269" s="0" t="s">
-        <v>776</v>
+        <v>154</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7986,16 +7972,19 @@
         <v>8</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C270" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="E270" s="0" t="s">
+        <v>775</v>
+      </c>
+      <c r="G270" s="0" t="s">
+        <v>776</v>
+      </c>
+      <c r="I270" s="0" t="s">
         <v>777</v>
-      </c>
-      <c r="E270" s="0" t="s">
-        <v>778</v>
-      </c>
-      <c r="I270" s="0" t="s">
-        <v>779</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8003,16 +7992,16 @@
         <v>8</v>
       </c>
       <c r="B271" s="1" t="s">
-        <v>649</v>
+        <v>778</v>
       </c>
       <c r="C271" s="1" t="s">
-        <v>153</v>
+        <v>779</v>
       </c>
       <c r="E271" s="0" t="s">
-        <v>153</v>
+        <v>780</v>
       </c>
       <c r="I271" s="0" t="s">
-        <v>154</v>
+        <v>781</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8020,19 +8009,16 @@
         <v>8</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>649</v>
+        <v>778</v>
       </c>
       <c r="C272" s="1" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
       <c r="E272" s="0" t="s">
-        <v>781</v>
-      </c>
-      <c r="G272" s="0" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="I272" s="0" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8040,7 +8026,7 @@
         <v>8</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>784</v>
+        <v>778</v>
       </c>
       <c r="C273" s="1" t="s">
         <v>785</v>
@@ -8057,7 +8043,7 @@
         <v>8</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>784</v>
+        <v>778</v>
       </c>
       <c r="C274" s="1" t="s">
         <v>788</v>
@@ -8074,7 +8060,7 @@
         <v>8</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>784</v>
+        <v>778</v>
       </c>
       <c r="C275" s="1" t="s">
         <v>791</v>
@@ -8091,7 +8077,7 @@
         <v>8</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>784</v>
+        <v>778</v>
       </c>
       <c r="C276" s="1" t="s">
         <v>794</v>
@@ -8108,7 +8094,7 @@
         <v>8</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>784</v>
+        <v>778</v>
       </c>
       <c r="C277" s="1" t="s">
         <v>797</v>
@@ -8125,7 +8111,7 @@
         <v>8</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>784</v>
+        <v>778</v>
       </c>
       <c r="C278" s="1" t="s">
         <v>800</v>
@@ -8142,7 +8128,7 @@
         <v>8</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>784</v>
+        <v>778</v>
       </c>
       <c r="C279" s="1" t="s">
         <v>803</v>
@@ -8159,7 +8145,7 @@
         <v>8</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>784</v>
+        <v>778</v>
       </c>
       <c r="C280" s="1" t="s">
         <v>806</v>
@@ -8176,7 +8162,7 @@
         <v>8</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>784</v>
+        <v>778</v>
       </c>
       <c r="C281" s="1" t="s">
         <v>809</v>
@@ -8193,7 +8179,7 @@
         <v>8</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>784</v>
+        <v>778</v>
       </c>
       <c r="C282" s="1" t="s">
         <v>812</v>
@@ -8210,7 +8196,7 @@
         <v>8</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>784</v>
+        <v>778</v>
       </c>
       <c r="C283" s="1" t="s">
         <v>815</v>
@@ -8227,7 +8213,7 @@
         <v>8</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>784</v>
+        <v>778</v>
       </c>
       <c r="C284" s="1" t="s">
         <v>818</v>
@@ -8244,7 +8230,7 @@
         <v>8</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>784</v>
+        <v>778</v>
       </c>
       <c r="C285" s="1" t="s">
         <v>821</v>
@@ -8261,7 +8247,7 @@
         <v>8</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>784</v>
+        <v>778</v>
       </c>
       <c r="C286" s="1" t="s">
         <v>824</v>
@@ -8278,7 +8264,7 @@
         <v>8</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>784</v>
+        <v>778</v>
       </c>
       <c r="C287" s="1" t="s">
         <v>827</v>
@@ -8295,7 +8281,7 @@
         <v>8</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>784</v>
+        <v>778</v>
       </c>
       <c r="C288" s="1" t="s">
         <v>830</v>
@@ -8312,7 +8298,7 @@
         <v>8</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>784</v>
+        <v>778</v>
       </c>
       <c r="C289" s="1" t="s">
         <v>833</v>
@@ -8329,7 +8315,7 @@
         <v>8</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>784</v>
+        <v>778</v>
       </c>
       <c r="C290" s="1" t="s">
         <v>836</v>
@@ -8346,7 +8332,7 @@
         <v>8</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>784</v>
+        <v>778</v>
       </c>
       <c r="C291" s="1" t="s">
         <v>839</v>
@@ -8363,7 +8349,7 @@
         <v>8</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>784</v>
+        <v>778</v>
       </c>
       <c r="C292" s="1" t="s">
         <v>842</v>
@@ -8380,7 +8366,7 @@
         <v>8</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>784</v>
+        <v>778</v>
       </c>
       <c r="C293" s="1" t="s">
         <v>845</v>
@@ -8397,16 +8383,16 @@
         <v>8</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>784</v>
+        <v>848</v>
       </c>
       <c r="C294" s="1" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="E294" s="0" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="I294" s="0" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8414,16 +8400,16 @@
         <v>8</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>784</v>
+        <v>848</v>
       </c>
       <c r="C295" s="1" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="E295" s="0" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="I295" s="0" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8431,16 +8417,16 @@
         <v>8</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="C296" s="1" t="s">
         <v>855</v>
       </c>
       <c r="E296" s="0" t="s">
+        <v>855</v>
+      </c>
+      <c r="I296" s="0" t="s">
         <v>856</v>
-      </c>
-      <c r="I296" s="0" t="s">
-        <v>857</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8448,16 +8434,16 @@
         <v>8</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="C297" s="1" t="s">
+        <v>857</v>
+      </c>
+      <c r="E297" s="0" t="s">
         <v>858</v>
       </c>
-      <c r="E297" s="0" t="s">
+      <c r="I297" s="0" t="s">
         <v>859</v>
-      </c>
-      <c r="I297" s="0" t="s">
-        <v>860</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8465,10 +8451,10 @@
         <v>8</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="C298" s="1" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="E298" s="0" t="s">
         <v>861</v>
@@ -8482,7 +8468,7 @@
         <v>8</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="C299" s="1" t="s">
         <v>863</v>
@@ -8499,7 +8485,7 @@
         <v>8</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="C300" s="1" t="s">
         <v>866</v>
@@ -8516,7 +8502,7 @@
         <v>8</v>
       </c>
       <c r="B301" s="1" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="C301" s="1" t="s">
         <v>869</v>
@@ -8533,7 +8519,7 @@
         <v>8</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="C302" s="1" t="s">
         <v>872</v>
@@ -8550,7 +8536,7 @@
         <v>8</v>
       </c>
       <c r="B303" s="1" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="C303" s="1" t="s">
         <v>875</v>
@@ -8567,7 +8553,7 @@
         <v>8</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="C304" s="1" t="s">
         <v>878</v>
@@ -8584,7 +8570,7 @@
         <v>8</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="C305" s="1" t="s">
         <v>881</v>
@@ -8596,20 +8582,20 @@
         <v>883</v>
       </c>
     </row>
-    <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="306" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B306" s="1" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="C306" s="1" t="s">
         <v>884</v>
       </c>
-      <c r="E306" s="0" t="s">
+      <c r="E306" s="2" t="s">
         <v>885</v>
       </c>
-      <c r="I306" s="0" t="s">
+      <c r="I306" s="2" t="s">
         <v>886</v>
       </c>
     </row>
@@ -8618,7 +8604,7 @@
         <v>8</v>
       </c>
       <c r="B307" s="1" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="C307" s="1" t="s">
         <v>887</v>
@@ -8630,20 +8616,20 @@
         <v>889</v>
       </c>
     </row>
-    <row r="308" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B308" s="1" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="C308" s="1" t="s">
         <v>890</v>
       </c>
-      <c r="E308" s="2" t="s">
+      <c r="E308" s="0" t="s">
         <v>891</v>
       </c>
-      <c r="I308" s="2" t="s">
+      <c r="I308" s="0" t="s">
         <v>892</v>
       </c>
     </row>
@@ -8652,7 +8638,7 @@
         <v>8</v>
       </c>
       <c r="B309" s="1" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="C309" s="1" t="s">
         <v>893</v>
@@ -8661,7 +8647,7 @@
         <v>894</v>
       </c>
       <c r="I309" s="0" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8669,16 +8655,16 @@
         <v>8</v>
       </c>
       <c r="B310" s="1" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="C310" s="1" t="s">
+        <v>895</v>
+      </c>
+      <c r="E310" s="0" t="s">
         <v>896</v>
       </c>
-      <c r="E310" s="0" t="s">
+      <c r="I310" s="0" t="s">
         <v>897</v>
-      </c>
-      <c r="I310" s="0" t="s">
-        <v>898</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8686,16 +8672,16 @@
         <v>8</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="C311" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="E311" s="0" t="s">
         <v>899</v>
       </c>
-      <c r="E311" s="0" t="s">
+      <c r="I311" s="0" t="s">
         <v>900</v>
-      </c>
-      <c r="I311" s="0" t="s">
-        <v>898</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8703,7 +8689,7 @@
         <v>8</v>
       </c>
       <c r="B312" s="1" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="C312" s="1" t="s">
         <v>901</v>
@@ -8720,7 +8706,7 @@
         <v>8</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="C313" s="1" t="s">
         <v>904</v>
@@ -8737,7 +8723,7 @@
         <v>8</v>
       </c>
       <c r="B314" s="1" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="C314" s="1" t="s">
         <v>907</v>
@@ -8754,7 +8740,7 @@
         <v>8</v>
       </c>
       <c r="B315" s="1" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="C315" s="1" t="s">
         <v>910</v>
@@ -8771,7 +8757,7 @@
         <v>8</v>
       </c>
       <c r="B316" s="1" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="C316" s="1" t="s">
         <v>913</v>
@@ -8788,7 +8774,7 @@
         <v>8</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="C317" s="1" t="s">
         <v>916</v>
@@ -8805,7 +8791,7 @@
         <v>8</v>
       </c>
       <c r="B318" s="1" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="C318" s="1" t="s">
         <v>919</v>
@@ -8822,7 +8808,7 @@
         <v>8</v>
       </c>
       <c r="B319" s="1" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="C319" s="1" t="s">
         <v>922</v>
@@ -8839,7 +8825,7 @@
         <v>8</v>
       </c>
       <c r="B320" s="1" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="C320" s="1" t="s">
         <v>925</v>
@@ -8856,7 +8842,7 @@
         <v>8</v>
       </c>
       <c r="B321" s="1" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="C321" s="1" t="s">
         <v>928</v>
@@ -8873,7 +8859,7 @@
         <v>8</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="C322" s="1" t="s">
         <v>931</v>
@@ -8890,7 +8876,7 @@
         <v>8</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="C323" s="1" t="s">
         <v>934</v>
@@ -8907,16 +8893,16 @@
         <v>8</v>
       </c>
       <c r="B324" s="1" t="s">
-        <v>854</v>
+        <v>937</v>
       </c>
       <c r="C324" s="1" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="E324" s="0" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="I324" s="0" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8924,16 +8910,16 @@
         <v>8</v>
       </c>
       <c r="B325" s="1" t="s">
-        <v>854</v>
+        <v>937</v>
       </c>
       <c r="C325" s="1" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="E325" s="0" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="I325" s="0" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8941,7 +8927,7 @@
         <v>8</v>
       </c>
       <c r="B326" s="1" t="s">
-        <v>943</v>
+        <v>937</v>
       </c>
       <c r="C326" s="1" t="s">
         <v>944</v>
@@ -8955,44 +8941,44 @@
     </row>
     <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="1" t="s">
-        <v>8</v>
+        <v>947</v>
       </c>
       <c r="B327" s="1" t="s">
-        <v>943</v>
+        <v>948</v>
       </c>
       <c r="C327" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E327" s="0" t="s">
-        <v>948</v>
+        <v>950</v>
       </c>
       <c r="I327" s="0" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="1" t="s">
-        <v>8</v>
+        <v>947</v>
       </c>
       <c r="B328" s="1" t="s">
-        <v>943</v>
+        <v>948</v>
       </c>
       <c r="C328" s="1" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="E328" s="0" t="s">
-        <v>951</v>
+        <v>953</v>
       </c>
       <c r="I328" s="0" t="s">
-        <v>952</v>
+        <v>954</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="1" t="s">
-        <v>953</v>
+        <v>947</v>
       </c>
       <c r="B329" s="1" t="s">
-        <v>954</v>
+        <v>948</v>
       </c>
       <c r="C329" s="1" t="s">
         <v>955</v>
@@ -9006,47 +8992,47 @@
     </row>
     <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="1" t="s">
-        <v>953</v>
+        <v>947</v>
       </c>
       <c r="B330" s="1" t="s">
-        <v>954</v>
+        <v>948</v>
       </c>
       <c r="C330" s="1" t="s">
         <v>958</v>
       </c>
       <c r="E330" s="0" t="s">
+        <v>958</v>
+      </c>
+      <c r="I330" s="0" t="s">
         <v>959</v>
-      </c>
-      <c r="I330" s="0" t="s">
-        <v>960</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="1" t="s">
-        <v>953</v>
+        <v>947</v>
       </c>
       <c r="B331" s="1" t="s">
-        <v>954</v>
+        <v>948</v>
       </c>
       <c r="C331" s="1" t="s">
+        <v>960</v>
+      </c>
+      <c r="E331" s="0" t="s">
         <v>961</v>
       </c>
-      <c r="E331" s="0" t="s">
+      <c r="I331" s="0" t="s">
         <v>962</v>
-      </c>
-      <c r="I331" s="0" t="s">
-        <v>963</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="1" t="s">
-        <v>953</v>
+        <v>947</v>
       </c>
       <c r="B332" s="1" t="s">
-        <v>954</v>
+        <v>948</v>
       </c>
       <c r="C332" s="1" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="E332" s="0" t="s">
         <v>964</v>
@@ -9057,10 +9043,10 @@
     </row>
     <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="1" t="s">
-        <v>953</v>
+        <v>947</v>
       </c>
       <c r="B333" s="1" t="s">
-        <v>954</v>
+        <v>948</v>
       </c>
       <c r="C333" s="1" t="s">
         <v>966</v>
@@ -9068,47 +9054,47 @@
       <c r="E333" s="0" t="s">
         <v>967</v>
       </c>
-      <c r="I333" s="0" t="s">
-        <v>968</v>
-      </c>
     </row>
     <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="1" t="s">
-        <v>953</v>
+        <v>947</v>
       </c>
       <c r="B334" s="1" t="s">
-        <v>954</v>
+        <v>948</v>
       </c>
       <c r="C334" s="1" t="s">
+        <v>968</v>
+      </c>
+      <c r="E334" s="0" t="s">
         <v>969</v>
       </c>
-      <c r="E334" s="0" t="s">
+      <c r="I334" s="0" t="s">
         <v>970</v>
-      </c>
-      <c r="I334" s="0" t="s">
-        <v>971</v>
       </c>
     </row>
     <row r="335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="1" t="s">
-        <v>953</v>
+        <v>947</v>
       </c>
       <c r="B335" s="1" t="s">
-        <v>954</v>
+        <v>948</v>
       </c>
       <c r="C335" s="1" t="s">
+        <v>971</v>
+      </c>
+      <c r="E335" s="0" t="s">
         <v>972</v>
       </c>
-      <c r="E335" s="0" t="s">
+      <c r="I335" s="0" t="s">
         <v>973</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="1" t="s">
-        <v>953</v>
+        <v>947</v>
       </c>
       <c r="B336" s="1" t="s">
-        <v>954</v>
+        <v>948</v>
       </c>
       <c r="C336" s="1" t="s">
         <v>974</v>
@@ -9122,10 +9108,10 @@
     </row>
     <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="1" t="s">
-        <v>953</v>
+        <v>947</v>
       </c>
       <c r="B337" s="1" t="s">
-        <v>954</v>
+        <v>948</v>
       </c>
       <c r="C337" s="1" t="s">
         <v>977</v>
@@ -9139,10 +9125,10 @@
     </row>
     <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="1" t="s">
-        <v>953</v>
+        <v>947</v>
       </c>
       <c r="B338" s="1" t="s">
-        <v>954</v>
+        <v>948</v>
       </c>
       <c r="C338" s="1" t="s">
         <v>980</v>
@@ -9156,10 +9142,10 @@
     </row>
     <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="1" t="s">
-        <v>953</v>
+        <v>947</v>
       </c>
       <c r="B339" s="1" t="s">
-        <v>954</v>
+        <v>948</v>
       </c>
       <c r="C339" s="1" t="s">
         <v>983</v>
@@ -9173,10 +9159,10 @@
     </row>
     <row r="340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="1" t="s">
-        <v>953</v>
+        <v>947</v>
       </c>
       <c r="B340" s="1" t="s">
-        <v>954</v>
+        <v>948</v>
       </c>
       <c r="C340" s="1" t="s">
         <v>986</v>
@@ -9190,61 +9176,61 @@
     </row>
     <row r="341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="1" t="s">
-        <v>953</v>
+        <v>947</v>
       </c>
       <c r="B341" s="1" t="s">
-        <v>954</v>
+        <v>948</v>
       </c>
       <c r="C341" s="1" t="s">
         <v>989</v>
       </c>
       <c r="E341" s="0" t="s">
-        <v>990</v>
-      </c>
-      <c r="I341" s="0" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="1" t="s">
-        <v>953</v>
+        <v>947</v>
       </c>
       <c r="B342" s="1" t="s">
-        <v>954</v>
+        <v>948</v>
       </c>
       <c r="C342" s="1" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="E342" s="0" t="s">
-        <v>993</v>
+        <v>990</v>
       </c>
       <c r="I342" s="0" t="s">
-        <v>994</v>
+        <v>991</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="1" t="s">
-        <v>953</v>
+        <v>947</v>
       </c>
       <c r="B343" s="1" t="s">
-        <v>954</v>
+        <v>948</v>
       </c>
       <c r="C343" s="1" t="s">
-        <v>995</v>
+        <v>992</v>
       </c>
       <c r="E343" s="0" t="s">
-        <v>995</v>
+        <v>993</v>
+      </c>
+      <c r="I343" s="0" t="s">
+        <v>994</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="1" t="s">
-        <v>953</v>
+        <v>947</v>
       </c>
       <c r="B344" s="1" t="s">
-        <v>954</v>
+        <v>948</v>
       </c>
       <c r="C344" s="1" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="E344" s="0" t="s">
         <v>996</v>
@@ -9255,10 +9241,10 @@
     </row>
     <row r="345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="1" t="s">
-        <v>953</v>
+        <v>947</v>
       </c>
       <c r="B345" s="1" t="s">
-        <v>954</v>
+        <v>948</v>
       </c>
       <c r="C345" s="1" t="s">
         <v>998</v>

</xml_diff>

<commit_message>
mathexample nl-NL now has more items
Also: update translations.
</commit_message>
<xml_diff>
--- a/docs/invariant/translations.xlsx
+++ b/docs/invariant/translations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1755" uniqueCount="1001">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1765" uniqueCount="1007">
   <si>
     <t xml:space="preserve">Project</t>
   </si>
@@ -2095,6 +2095,24 @@
     <t xml:space="preserve">Het verwijderen van bestanden (met [{0}] in de volledige bestandsnaam) uit Dropbox is mislukt. Een waarschijnlijke oorzaak: geen internetverbinding of een bestand is in gebruik. Learn8 zal het opnieuw proberen bij de volgende synchronisatie.</t>
   </si>
   <si>
+    <t xml:space="preserve">Sync_in_progress_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sync in progress...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Synchronisatie bezig...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sync_finished_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sync finished.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Synchronisatie voltooid.</t>
+  </si>
+  <si>
     <t xml:space="preserve">_LanguageResources\Settings</t>
   </si>
   <si>
@@ -3175,7 +3193,7 @@
     <t xml:space="preserve">Share a Learn8 package or share a link to another website</t>
   </si>
   <si>
-    <t xml:space="preserve">Een Learn8 pakketje of een link naar een andere website delen</t>
+    <t xml:space="preserve">Deel een Learn8 pakketje of een link naar een andere website</t>
   </si>
   <si>
     <t xml:space="preserve">Sharing_Info</t>
@@ -3289,7 +3307,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I345"/>
+  <dimension ref="A1:I347"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
@@ -7231,16 +7249,16 @@
         <v>8</v>
       </c>
       <c r="B228" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="C228" s="1" t="s">
         <v>643</v>
       </c>
-      <c r="C228" s="1" t="s">
+      <c r="E228" s="0" t="s">
         <v>644</v>
       </c>
-      <c r="E228" s="0" t="s">
+      <c r="I228" s="0" t="s">
         <v>645</v>
-      </c>
-      <c r="I228" s="0" t="s">
-        <v>646</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7248,16 +7266,16 @@
         <v>8</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>643</v>
+        <v>514</v>
       </c>
       <c r="C229" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="E229" s="0" t="s">
         <v>647</v>
       </c>
-      <c r="E229" s="0" t="s">
+      <c r="I229" s="0" t="s">
         <v>648</v>
-      </c>
-      <c r="I229" s="0" t="s">
-        <v>649</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7265,7 +7283,7 @@
         <v>8</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C230" s="1" t="s">
         <v>650</v>
@@ -7282,7 +7300,7 @@
         <v>8</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C231" s="1" t="s">
         <v>653</v>
@@ -7299,7 +7317,7 @@
         <v>8</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C232" s="1" t="s">
         <v>656</v>
@@ -7316,7 +7334,7 @@
         <v>8</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C233" s="1" t="s">
         <v>659</v>
@@ -7324,14 +7342,8 @@
       <c r="E233" s="0" t="s">
         <v>660</v>
       </c>
-      <c r="F233" s="0" t="s">
+      <c r="I233" s="0" t="s">
         <v>661</v>
-      </c>
-      <c r="G233" s="0" t="s">
-        <v>662</v>
-      </c>
-      <c r="I233" s="0" t="s">
-        <v>663</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7339,22 +7351,16 @@
         <v>8</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C234" s="1" t="s">
+        <v>662</v>
+      </c>
+      <c r="E234" s="0" t="s">
+        <v>663</v>
+      </c>
+      <c r="I234" s="0" t="s">
         <v>664</v>
-      </c>
-      <c r="E234" s="0" t="s">
-        <v>664</v>
-      </c>
-      <c r="F234" s="0" t="s">
-        <v>665</v>
-      </c>
-      <c r="G234" s="0" t="s">
-        <v>666</v>
-      </c>
-      <c r="I234" s="0" t="s">
-        <v>667</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7362,16 +7368,22 @@
         <v>8</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C235" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="E235" s="0" t="s">
+        <v>666</v>
+      </c>
+      <c r="F235" s="0" t="s">
+        <v>667</v>
+      </c>
+      <c r="G235" s="0" t="s">
         <v>668</v>
       </c>
-      <c r="E235" s="0" t="s">
+      <c r="I235" s="0" t="s">
         <v>669</v>
-      </c>
-      <c r="I235" s="0" t="s">
-        <v>670</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7379,22 +7391,22 @@
         <v>8</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C236" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="E236" s="0" t="s">
+        <v>670</v>
+      </c>
+      <c r="F236" s="0" t="s">
         <v>671</v>
       </c>
-      <c r="E236" s="0" t="s">
+      <c r="G236" s="0" t="s">
         <v>672</v>
       </c>
-      <c r="F236" s="0" t="s">
+      <c r="I236" s="0" t="s">
         <v>673</v>
-      </c>
-      <c r="G236" s="0" t="s">
-        <v>674</v>
-      </c>
-      <c r="I236" s="0" t="s">
-        <v>675</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7402,16 +7414,16 @@
         <v>8</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C237" s="1" t="s">
+        <v>674</v>
+      </c>
+      <c r="E237" s="0" t="s">
+        <v>675</v>
+      </c>
+      <c r="I237" s="0" t="s">
         <v>676</v>
-      </c>
-      <c r="E237" s="0" t="s">
-        <v>677</v>
-      </c>
-      <c r="I237" s="0" t="s">
-        <v>678</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7419,12 +7431,18 @@
         <v>8</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C238" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="E238" s="0" t="s">
+        <v>678</v>
+      </c>
+      <c r="F238" s="0" t="s">
         <v>679</v>
       </c>
-      <c r="E238" s="0" t="s">
+      <c r="G238" s="0" t="s">
         <v>680</v>
       </c>
       <c r="I238" s="0" t="s">
@@ -7436,7 +7454,7 @@
         <v>8</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C239" s="1" t="s">
         <v>682</v>
@@ -7444,14 +7462,8 @@
       <c r="E239" s="0" t="s">
         <v>683</v>
       </c>
-      <c r="F239" s="0" t="s">
+      <c r="I239" s="0" t="s">
         <v>684</v>
-      </c>
-      <c r="G239" s="0" t="s">
-        <v>685</v>
-      </c>
-      <c r="I239" s="0" t="s">
-        <v>686</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7459,19 +7471,16 @@
         <v>8</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C240" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="E240" s="0" t="s">
+        <v>686</v>
+      </c>
+      <c r="I240" s="0" t="s">
         <v>687</v>
-      </c>
-      <c r="E240" s="0" t="s">
-        <v>688</v>
-      </c>
-      <c r="G240" s="0" t="s">
-        <v>689</v>
-      </c>
-      <c r="I240" s="0" t="s">
-        <v>690</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7479,32 +7488,41 @@
         <v>8</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C241" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="E241" s="0" t="s">
+        <v>689</v>
+      </c>
+      <c r="F241" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="G241" s="0" t="s">
         <v>691</v>
       </c>
-      <c r="E241" s="0" t="s">
+      <c r="I241" s="0" t="s">
         <v>692</v>
       </c>
-      <c r="I241" s="0" t="s">
+    </row>
+    <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A242" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B242" s="1" t="s">
+        <v>649</v>
+      </c>
+      <c r="C242" s="1" t="s">
         <v>693</v>
       </c>
-    </row>
-    <row r="242" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A242" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B242" s="1" t="s">
-        <v>643</v>
-      </c>
-      <c r="C242" s="1" t="s">
+      <c r="E242" s="0" t="s">
         <v>694</v>
       </c>
-      <c r="E242" s="2" t="s">
+      <c r="G242" s="0" t="s">
         <v>695</v>
       </c>
-      <c r="I242" s="2" t="s">
+      <c r="I242" s="0" t="s">
         <v>696</v>
       </c>
     </row>
@@ -7513,7 +7531,7 @@
         <v>8</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C243" s="1" t="s">
         <v>697</v>
@@ -7525,88 +7543,88 @@
         <v>699</v>
       </c>
     </row>
-    <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="244" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C244" s="1" t="s">
         <v>700</v>
       </c>
-      <c r="E244" s="0" t="s">
+      <c r="E244" s="2" t="s">
         <v>701</v>
       </c>
-      <c r="I244" s="0" t="s">
+      <c r="I244" s="2" t="s">
         <v>702</v>
       </c>
     </row>
-    <row r="245" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C245" s="1" t="s">
         <v>703</v>
       </c>
-      <c r="E245" s="2" t="s">
+      <c r="E245" s="0" t="s">
         <v>704</v>
       </c>
-      <c r="I245" s="2" t="s">
+      <c r="I245" s="0" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="246" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C246" s="1" t="s">
         <v>706</v>
       </c>
-      <c r="E246" s="2" t="s">
+      <c r="E246" s="0" t="s">
         <v>707</v>
       </c>
-      <c r="I246" s="2" t="s">
+      <c r="I246" s="0" t="s">
         <v>708</v>
       </c>
     </row>
-    <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="247" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C247" s="1" t="s">
         <v>709</v>
       </c>
-      <c r="E247" s="0" t="s">
+      <c r="E247" s="2" t="s">
         <v>710</v>
       </c>
-      <c r="I247" s="0" t="s">
+      <c r="I247" s="2" t="s">
         <v>711</v>
       </c>
     </row>
-    <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="248" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C248" s="1" t="s">
         <v>712</v>
       </c>
-      <c r="E248" s="0" t="s">
+      <c r="E248" s="2" t="s">
         <v>713</v>
       </c>
-      <c r="I248" s="0" t="s">
+      <c r="I248" s="2" t="s">
         <v>714</v>
       </c>
     </row>
@@ -7615,7 +7633,7 @@
         <v>8</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C249" s="1" t="s">
         <v>715</v>
@@ -7632,7 +7650,7 @@
         <v>8</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C250" s="1" t="s">
         <v>718</v>
@@ -7649,7 +7667,7 @@
         <v>8</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C251" s="1" t="s">
         <v>721</v>
@@ -7666,7 +7684,7 @@
         <v>8</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C252" s="1" t="s">
         <v>724</v>
@@ -7683,7 +7701,7 @@
         <v>8</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C253" s="1" t="s">
         <v>727</v>
@@ -7700,7 +7718,7 @@
         <v>8</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C254" s="1" t="s">
         <v>730</v>
@@ -7717,7 +7735,7 @@
         <v>8</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C255" s="1" t="s">
         <v>733</v>
@@ -7734,7 +7752,7 @@
         <v>8</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C256" s="1" t="s">
         <v>736</v>
@@ -7751,7 +7769,7 @@
         <v>8</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C257" s="1" t="s">
         <v>739</v>
@@ -7768,7 +7786,7 @@
         <v>8</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C258" s="1" t="s">
         <v>742</v>
@@ -7785,7 +7803,7 @@
         <v>8</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C259" s="1" t="s">
         <v>745</v>
@@ -7802,7 +7820,7 @@
         <v>8</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C260" s="1" t="s">
         <v>748</v>
@@ -7819,7 +7837,7 @@
         <v>8</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C261" s="1" t="s">
         <v>751</v>
@@ -7836,7 +7854,7 @@
         <v>8</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C262" s="1" t="s">
         <v>754</v>
@@ -7853,7 +7871,7 @@
         <v>8</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C263" s="1" t="s">
         <v>757</v>
@@ -7862,7 +7880,7 @@
         <v>758</v>
       </c>
       <c r="I263" s="0" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7870,16 +7888,16 @@
         <v>8</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C264" s="1" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="E264" s="0" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="I264" s="0" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7887,13 +7905,13 @@
         <v>8</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C265" s="1" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="E265" s="0" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="I265" s="0" t="s">
         <v>764</v>
@@ -7904,7 +7922,7 @@
         <v>8</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C266" s="1" t="s">
         <v>765</v>
@@ -7921,7 +7939,7 @@
         <v>8</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C267" s="1" t="s">
         <v>768</v>
@@ -7938,7 +7956,7 @@
         <v>8</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C268" s="1" t="s">
         <v>771</v>
@@ -7955,16 +7973,16 @@
         <v>8</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C269" s="1" t="s">
-        <v>153</v>
+        <v>774</v>
       </c>
       <c r="E269" s="0" t="s">
-        <v>153</v>
+        <v>775</v>
       </c>
       <c r="I269" s="0" t="s">
-        <v>154</v>
+        <v>776</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7972,19 +7990,16 @@
         <v>8</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C270" s="1" t="s">
-        <v>774</v>
+        <v>777</v>
       </c>
       <c r="E270" s="0" t="s">
-        <v>775</v>
-      </c>
-      <c r="G270" s="0" t="s">
-        <v>776</v>
+        <v>778</v>
       </c>
       <c r="I270" s="0" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7992,16 +8007,16 @@
         <v>8</v>
       </c>
       <c r="B271" s="1" t="s">
-        <v>778</v>
+        <v>649</v>
       </c>
       <c r="C271" s="1" t="s">
-        <v>779</v>
+        <v>153</v>
       </c>
       <c r="E271" s="0" t="s">
-        <v>780</v>
+        <v>153</v>
       </c>
       <c r="I271" s="0" t="s">
-        <v>781</v>
+        <v>154</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8009,16 +8024,19 @@
         <v>8</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>778</v>
+        <v>649</v>
       </c>
       <c r="C272" s="1" t="s">
+        <v>780</v>
+      </c>
+      <c r="E272" s="0" t="s">
+        <v>781</v>
+      </c>
+      <c r="G272" s="0" t="s">
         <v>782</v>
       </c>
-      <c r="E272" s="0" t="s">
+      <c r="I272" s="0" t="s">
         <v>783</v>
-      </c>
-      <c r="I272" s="0" t="s">
-        <v>784</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8026,7 +8044,7 @@
         <v>8</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>778</v>
+        <v>784</v>
       </c>
       <c r="C273" s="1" t="s">
         <v>785</v>
@@ -8043,7 +8061,7 @@
         <v>8</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>778</v>
+        <v>784</v>
       </c>
       <c r="C274" s="1" t="s">
         <v>788</v>
@@ -8060,7 +8078,7 @@
         <v>8</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>778</v>
+        <v>784</v>
       </c>
       <c r="C275" s="1" t="s">
         <v>791</v>
@@ -8077,7 +8095,7 @@
         <v>8</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>778</v>
+        <v>784</v>
       </c>
       <c r="C276" s="1" t="s">
         <v>794</v>
@@ -8094,7 +8112,7 @@
         <v>8</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>778</v>
+        <v>784</v>
       </c>
       <c r="C277" s="1" t="s">
         <v>797</v>
@@ -8111,7 +8129,7 @@
         <v>8</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>778</v>
+        <v>784</v>
       </c>
       <c r="C278" s="1" t="s">
         <v>800</v>
@@ -8128,7 +8146,7 @@
         <v>8</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>778</v>
+        <v>784</v>
       </c>
       <c r="C279" s="1" t="s">
         <v>803</v>
@@ -8145,7 +8163,7 @@
         <v>8</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>778</v>
+        <v>784</v>
       </c>
       <c r="C280" s="1" t="s">
         <v>806</v>
@@ -8162,7 +8180,7 @@
         <v>8</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>778</v>
+        <v>784</v>
       </c>
       <c r="C281" s="1" t="s">
         <v>809</v>
@@ -8179,7 +8197,7 @@
         <v>8</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>778</v>
+        <v>784</v>
       </c>
       <c r="C282" s="1" t="s">
         <v>812</v>
@@ -8196,7 +8214,7 @@
         <v>8</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>778</v>
+        <v>784</v>
       </c>
       <c r="C283" s="1" t="s">
         <v>815</v>
@@ -8213,7 +8231,7 @@
         <v>8</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>778</v>
+        <v>784</v>
       </c>
       <c r="C284" s="1" t="s">
         <v>818</v>
@@ -8230,7 +8248,7 @@
         <v>8</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>778</v>
+        <v>784</v>
       </c>
       <c r="C285" s="1" t="s">
         <v>821</v>
@@ -8247,7 +8265,7 @@
         <v>8</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>778</v>
+        <v>784</v>
       </c>
       <c r="C286" s="1" t="s">
         <v>824</v>
@@ -8264,7 +8282,7 @@
         <v>8</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>778</v>
+        <v>784</v>
       </c>
       <c r="C287" s="1" t="s">
         <v>827</v>
@@ -8281,7 +8299,7 @@
         <v>8</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>778</v>
+        <v>784</v>
       </c>
       <c r="C288" s="1" t="s">
         <v>830</v>
@@ -8298,7 +8316,7 @@
         <v>8</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>778</v>
+        <v>784</v>
       </c>
       <c r="C289" s="1" t="s">
         <v>833</v>
@@ -8315,7 +8333,7 @@
         <v>8</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>778</v>
+        <v>784</v>
       </c>
       <c r="C290" s="1" t="s">
         <v>836</v>
@@ -8332,7 +8350,7 @@
         <v>8</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>778</v>
+        <v>784</v>
       </c>
       <c r="C291" s="1" t="s">
         <v>839</v>
@@ -8349,7 +8367,7 @@
         <v>8</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>778</v>
+        <v>784</v>
       </c>
       <c r="C292" s="1" t="s">
         <v>842</v>
@@ -8366,7 +8384,7 @@
         <v>8</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>778</v>
+        <v>784</v>
       </c>
       <c r="C293" s="1" t="s">
         <v>845</v>
@@ -8383,16 +8401,16 @@
         <v>8</v>
       </c>
       <c r="B294" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="C294" s="1" t="s">
         <v>848</v>
       </c>
-      <c r="C294" s="1" t="s">
+      <c r="E294" s="0" t="s">
         <v>849</v>
       </c>
-      <c r="E294" s="0" t="s">
+      <c r="I294" s="0" t="s">
         <v>850</v>
-      </c>
-      <c r="I294" s="0" t="s">
-        <v>851</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8400,16 +8418,16 @@
         <v>8</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>848</v>
+        <v>784</v>
       </c>
       <c r="C295" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="E295" s="0" t="s">
         <v>852</v>
       </c>
-      <c r="E295" s="0" t="s">
+      <c r="I295" s="0" t="s">
         <v>853</v>
-      </c>
-      <c r="I295" s="0" t="s">
-        <v>854</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8417,16 +8435,16 @@
         <v>8</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>848</v>
+        <v>854</v>
       </c>
       <c r="C296" s="1" t="s">
         <v>855</v>
       </c>
       <c r="E296" s="0" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="I296" s="0" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8434,16 +8452,16 @@
         <v>8</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>848</v>
+        <v>854</v>
       </c>
       <c r="C297" s="1" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="E297" s="0" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="I297" s="0" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8451,10 +8469,10 @@
         <v>8</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>848</v>
+        <v>854</v>
       </c>
       <c r="C298" s="1" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="E298" s="0" t="s">
         <v>861</v>
@@ -8468,7 +8486,7 @@
         <v>8</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>848</v>
+        <v>854</v>
       </c>
       <c r="C299" s="1" t="s">
         <v>863</v>
@@ -8485,7 +8503,7 @@
         <v>8</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>848</v>
+        <v>854</v>
       </c>
       <c r="C300" s="1" t="s">
         <v>866</v>
@@ -8502,7 +8520,7 @@
         <v>8</v>
       </c>
       <c r="B301" s="1" t="s">
-        <v>848</v>
+        <v>854</v>
       </c>
       <c r="C301" s="1" t="s">
         <v>869</v>
@@ -8519,7 +8537,7 @@
         <v>8</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>848</v>
+        <v>854</v>
       </c>
       <c r="C302" s="1" t="s">
         <v>872</v>
@@ -8536,7 +8554,7 @@
         <v>8</v>
       </c>
       <c r="B303" s="1" t="s">
-        <v>848</v>
+        <v>854</v>
       </c>
       <c r="C303" s="1" t="s">
         <v>875</v>
@@ -8553,7 +8571,7 @@
         <v>8</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>848</v>
+        <v>854</v>
       </c>
       <c r="C304" s="1" t="s">
         <v>878</v>
@@ -8570,7 +8588,7 @@
         <v>8</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>848</v>
+        <v>854</v>
       </c>
       <c r="C305" s="1" t="s">
         <v>881</v>
@@ -8582,20 +8600,20 @@
         <v>883</v>
       </c>
     </row>
-    <row r="306" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B306" s="1" t="s">
-        <v>848</v>
+        <v>854</v>
       </c>
       <c r="C306" s="1" t="s">
         <v>884</v>
       </c>
-      <c r="E306" s="2" t="s">
+      <c r="E306" s="0" t="s">
         <v>885</v>
       </c>
-      <c r="I306" s="2" t="s">
+      <c r="I306" s="0" t="s">
         <v>886</v>
       </c>
     </row>
@@ -8604,7 +8622,7 @@
         <v>8</v>
       </c>
       <c r="B307" s="1" t="s">
-        <v>848</v>
+        <v>854</v>
       </c>
       <c r="C307" s="1" t="s">
         <v>887</v>
@@ -8616,20 +8634,20 @@
         <v>889</v>
       </c>
     </row>
-    <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="308" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B308" s="1" t="s">
-        <v>848</v>
+        <v>854</v>
       </c>
       <c r="C308" s="1" t="s">
         <v>890</v>
       </c>
-      <c r="E308" s="0" t="s">
+      <c r="E308" s="2" t="s">
         <v>891</v>
       </c>
-      <c r="I308" s="0" t="s">
+      <c r="I308" s="2" t="s">
         <v>892</v>
       </c>
     </row>
@@ -8638,7 +8656,7 @@
         <v>8</v>
       </c>
       <c r="B309" s="1" t="s">
-        <v>848</v>
+        <v>854</v>
       </c>
       <c r="C309" s="1" t="s">
         <v>893</v>
@@ -8647,7 +8665,7 @@
         <v>894</v>
       </c>
       <c r="I309" s="0" t="s">
-        <v>892</v>
+        <v>895</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8655,16 +8673,16 @@
         <v>8</v>
       </c>
       <c r="B310" s="1" t="s">
-        <v>848</v>
+        <v>854</v>
       </c>
       <c r="C310" s="1" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="E310" s="0" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="I310" s="0" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8672,16 +8690,16 @@
         <v>8</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>848</v>
+        <v>854</v>
       </c>
       <c r="C311" s="1" t="s">
+        <v>899</v>
+      </c>
+      <c r="E311" s="0" t="s">
+        <v>900</v>
+      </c>
+      <c r="I311" s="0" t="s">
         <v>898</v>
-      </c>
-      <c r="E311" s="0" t="s">
-        <v>899</v>
-      </c>
-      <c r="I311" s="0" t="s">
-        <v>900</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8689,7 +8707,7 @@
         <v>8</v>
       </c>
       <c r="B312" s="1" t="s">
-        <v>848</v>
+        <v>854</v>
       </c>
       <c r="C312" s="1" t="s">
         <v>901</v>
@@ -8706,7 +8724,7 @@
         <v>8</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>848</v>
+        <v>854</v>
       </c>
       <c r="C313" s="1" t="s">
         <v>904</v>
@@ -8723,7 +8741,7 @@
         <v>8</v>
       </c>
       <c r="B314" s="1" t="s">
-        <v>848</v>
+        <v>854</v>
       </c>
       <c r="C314" s="1" t="s">
         <v>907</v>
@@ -8740,7 +8758,7 @@
         <v>8</v>
       </c>
       <c r="B315" s="1" t="s">
-        <v>848</v>
+        <v>854</v>
       </c>
       <c r="C315" s="1" t="s">
         <v>910</v>
@@ -8757,7 +8775,7 @@
         <v>8</v>
       </c>
       <c r="B316" s="1" t="s">
-        <v>848</v>
+        <v>854</v>
       </c>
       <c r="C316" s="1" t="s">
         <v>913</v>
@@ -8774,7 +8792,7 @@
         <v>8</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>848</v>
+        <v>854</v>
       </c>
       <c r="C317" s="1" t="s">
         <v>916</v>
@@ -8791,7 +8809,7 @@
         <v>8</v>
       </c>
       <c r="B318" s="1" t="s">
-        <v>848</v>
+        <v>854</v>
       </c>
       <c r="C318" s="1" t="s">
         <v>919</v>
@@ -8808,7 +8826,7 @@
         <v>8</v>
       </c>
       <c r="B319" s="1" t="s">
-        <v>848</v>
+        <v>854</v>
       </c>
       <c r="C319" s="1" t="s">
         <v>922</v>
@@ -8825,7 +8843,7 @@
         <v>8</v>
       </c>
       <c r="B320" s="1" t="s">
-        <v>848</v>
+        <v>854</v>
       </c>
       <c r="C320" s="1" t="s">
         <v>925</v>
@@ -8842,7 +8860,7 @@
         <v>8</v>
       </c>
       <c r="B321" s="1" t="s">
-        <v>848</v>
+        <v>854</v>
       </c>
       <c r="C321" s="1" t="s">
         <v>928</v>
@@ -8859,7 +8877,7 @@
         <v>8</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>848</v>
+        <v>854</v>
       </c>
       <c r="C322" s="1" t="s">
         <v>931</v>
@@ -8876,7 +8894,7 @@
         <v>8</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>848</v>
+        <v>854</v>
       </c>
       <c r="C323" s="1" t="s">
         <v>934</v>
@@ -8893,16 +8911,16 @@
         <v>8</v>
       </c>
       <c r="B324" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="C324" s="1" t="s">
         <v>937</v>
       </c>
-      <c r="C324" s="1" t="s">
+      <c r="E324" s="0" t="s">
         <v>938</v>
       </c>
-      <c r="E324" s="0" t="s">
+      <c r="I324" s="0" t="s">
         <v>939</v>
-      </c>
-      <c r="I324" s="0" t="s">
-        <v>940</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8910,16 +8928,16 @@
         <v>8</v>
       </c>
       <c r="B325" s="1" t="s">
-        <v>937</v>
+        <v>854</v>
       </c>
       <c r="C325" s="1" t="s">
+        <v>940</v>
+      </c>
+      <c r="E325" s="0" t="s">
         <v>941</v>
       </c>
-      <c r="E325" s="0" t="s">
+      <c r="I325" s="0" t="s">
         <v>942</v>
-      </c>
-      <c r="I325" s="0" t="s">
-        <v>943</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8927,7 +8945,7 @@
         <v>8</v>
       </c>
       <c r="B326" s="1" t="s">
-        <v>937</v>
+        <v>943</v>
       </c>
       <c r="C326" s="1" t="s">
         <v>944</v>
@@ -8941,44 +8959,44 @@
     </row>
     <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B327" s="1" t="s">
+        <v>943</v>
+      </c>
+      <c r="C327" s="1" t="s">
         <v>947</v>
       </c>
-      <c r="B327" s="1" t="s">
+      <c r="E327" s="0" t="s">
         <v>948</v>
       </c>
-      <c r="C327" s="1" t="s">
+      <c r="I327" s="0" t="s">
         <v>949</v>
-      </c>
-      <c r="E327" s="0" t="s">
-        <v>950</v>
-      </c>
-      <c r="I327" s="0" t="s">
-        <v>951</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="1" t="s">
-        <v>947</v>
+        <v>8</v>
       </c>
       <c r="B328" s="1" t="s">
-        <v>948</v>
+        <v>943</v>
       </c>
       <c r="C328" s="1" t="s">
+        <v>950</v>
+      </c>
+      <c r="E328" s="0" t="s">
+        <v>951</v>
+      </c>
+      <c r="I328" s="0" t="s">
         <v>952</v>
-      </c>
-      <c r="E328" s="0" t="s">
-        <v>953</v>
-      </c>
-      <c r="I328" s="0" t="s">
-        <v>954</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="1" t="s">
-        <v>947</v>
+        <v>953</v>
       </c>
       <c r="B329" s="1" t="s">
-        <v>948</v>
+        <v>954</v>
       </c>
       <c r="C329" s="1" t="s">
         <v>955</v>
@@ -8992,47 +9010,47 @@
     </row>
     <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="1" t="s">
-        <v>947</v>
+        <v>953</v>
       </c>
       <c r="B330" s="1" t="s">
-        <v>948</v>
+        <v>954</v>
       </c>
       <c r="C330" s="1" t="s">
         <v>958</v>
       </c>
       <c r="E330" s="0" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="I330" s="0" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="1" t="s">
-        <v>947</v>
+        <v>953</v>
       </c>
       <c r="B331" s="1" t="s">
-        <v>948</v>
+        <v>954</v>
       </c>
       <c r="C331" s="1" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="E331" s="0" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="I331" s="0" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="1" t="s">
-        <v>947</v>
+        <v>953</v>
       </c>
       <c r="B332" s="1" t="s">
-        <v>948</v>
+        <v>954</v>
       </c>
       <c r="C332" s="1" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="E332" s="0" t="s">
         <v>964</v>
@@ -9043,10 +9061,10 @@
     </row>
     <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="1" t="s">
-        <v>947</v>
+        <v>953</v>
       </c>
       <c r="B333" s="1" t="s">
-        <v>948</v>
+        <v>954</v>
       </c>
       <c r="C333" s="1" t="s">
         <v>966</v>
@@ -9054,47 +9072,47 @@
       <c r="E333" s="0" t="s">
         <v>967</v>
       </c>
+      <c r="I333" s="0" t="s">
+        <v>968</v>
+      </c>
     </row>
     <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="1" t="s">
-        <v>947</v>
+        <v>953</v>
       </c>
       <c r="B334" s="1" t="s">
-        <v>948</v>
+        <v>954</v>
       </c>
       <c r="C334" s="1" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="E334" s="0" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="I334" s="0" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
     </row>
     <row r="335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="1" t="s">
-        <v>947</v>
+        <v>953</v>
       </c>
       <c r="B335" s="1" t="s">
-        <v>948</v>
+        <v>954</v>
       </c>
       <c r="C335" s="1" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="E335" s="0" t="s">
-        <v>972</v>
-      </c>
-      <c r="I335" s="0" t="s">
         <v>973</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="1" t="s">
-        <v>947</v>
+        <v>953</v>
       </c>
       <c r="B336" s="1" t="s">
-        <v>948</v>
+        <v>954</v>
       </c>
       <c r="C336" s="1" t="s">
         <v>974</v>
@@ -9108,10 +9126,10 @@
     </row>
     <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="1" t="s">
-        <v>947</v>
+        <v>953</v>
       </c>
       <c r="B337" s="1" t="s">
-        <v>948</v>
+        <v>954</v>
       </c>
       <c r="C337" s="1" t="s">
         <v>977</v>
@@ -9125,10 +9143,10 @@
     </row>
     <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="1" t="s">
-        <v>947</v>
+        <v>953</v>
       </c>
       <c r="B338" s="1" t="s">
-        <v>948</v>
+        <v>954</v>
       </c>
       <c r="C338" s="1" t="s">
         <v>980</v>
@@ -9142,10 +9160,10 @@
     </row>
     <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="1" t="s">
-        <v>947</v>
+        <v>953</v>
       </c>
       <c r="B339" s="1" t="s">
-        <v>948</v>
+        <v>954</v>
       </c>
       <c r="C339" s="1" t="s">
         <v>983</v>
@@ -9159,10 +9177,10 @@
     </row>
     <row r="340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="1" t="s">
-        <v>947</v>
+        <v>953</v>
       </c>
       <c r="B340" s="1" t="s">
-        <v>948</v>
+        <v>954</v>
       </c>
       <c r="C340" s="1" t="s">
         <v>986</v>
@@ -9176,61 +9194,61 @@
     </row>
     <row r="341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="1" t="s">
-        <v>947</v>
+        <v>953</v>
       </c>
       <c r="B341" s="1" t="s">
-        <v>948</v>
+        <v>954</v>
       </c>
       <c r="C341" s="1" t="s">
         <v>989</v>
       </c>
       <c r="E341" s="0" t="s">
-        <v>989</v>
+        <v>990</v>
+      </c>
+      <c r="I341" s="0" t="s">
+        <v>991</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="1" t="s">
-        <v>947</v>
+        <v>953</v>
       </c>
       <c r="B342" s="1" t="s">
-        <v>948</v>
+        <v>954</v>
       </c>
       <c r="C342" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E342" s="0" t="s">
-        <v>990</v>
+        <v>993</v>
       </c>
       <c r="I342" s="0" t="s">
-        <v>991</v>
+        <v>994</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="1" t="s">
-        <v>947</v>
+        <v>953</v>
       </c>
       <c r="B343" s="1" t="s">
-        <v>948</v>
+        <v>954</v>
       </c>
       <c r="C343" s="1" t="s">
-        <v>992</v>
+        <v>995</v>
       </c>
       <c r="E343" s="0" t="s">
-        <v>993</v>
-      </c>
-      <c r="I343" s="0" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="1" t="s">
-        <v>947</v>
+        <v>953</v>
       </c>
       <c r="B344" s="1" t="s">
-        <v>948</v>
+        <v>954</v>
       </c>
       <c r="C344" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E344" s="0" t="s">
         <v>996</v>
@@ -9241,10 +9259,10 @@
     </row>
     <row r="345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="1" t="s">
-        <v>947</v>
+        <v>953</v>
       </c>
       <c r="B345" s="1" t="s">
-        <v>948</v>
+        <v>954</v>
       </c>
       <c r="C345" s="1" t="s">
         <v>998</v>
@@ -9254,6 +9272,40 @@
       </c>
       <c r="I345" s="0" t="s">
         <v>1000</v>
+      </c>
+    </row>
+    <row r="346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A346" s="1" t="s">
+        <v>953</v>
+      </c>
+      <c r="B346" s="1" t="s">
+        <v>954</v>
+      </c>
+      <c r="C346" s="1" t="s">
+        <v>1001</v>
+      </c>
+      <c r="E346" s="0" t="s">
+        <v>1002</v>
+      </c>
+      <c r="I346" s="0" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A347" s="1" t="s">
+        <v>953</v>
+      </c>
+      <c r="B347" s="1" t="s">
+        <v>954</v>
+      </c>
+      <c r="C347" s="1" t="s">
+        <v>1004</v>
+      </c>
+      <c r="E347" s="0" t="s">
+        <v>1005</v>
+      </c>
+      <c r="I347" s="0" t="s">
+        <v>1006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use the text "Learn8 items" instead of "Learn8 package"
</commit_message>
<xml_diff>
--- a/docs/invariant/translations.xlsx
+++ b/docs/invariant/translations.xlsx
@@ -2095,6 +2095,15 @@
     <t xml:space="preserve">Het verwijderen van bestanden (met [{0}] in de volledige bestandsnaam) uit Dropbox is mislukt. Een waarschijnlijke oorzaak: geen internetverbinding of een bestand is in gebruik. Learn8 zal het opnieuw proberen bij de volgende synchronisatie.</t>
   </si>
   <si>
+    <t xml:space="preserve">Sync_finished_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sync finished.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Synchronisatie voltooid.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sync_in_progress_</t>
   </si>
   <si>
@@ -2102,15 +2111,6 @@
   </si>
   <si>
     <t xml:space="preserve">Synchronisatie bezig...</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sync_finished_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sync finished.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Synchronisatie voltooid.</t>
   </si>
   <si>
     <t xml:space="preserve">_LanguageResources\Settings</t>
@@ -3190,19 +3190,19 @@
     <t xml:space="preserve">Sharing_a_package_or_other_website</t>
   </si>
   <si>
-    <t xml:space="preserve">Share a Learn8 package or share a link to another website</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deel een Learn8 pakketje of een link naar een andere website</t>
+    <t xml:space="preserve">Share Learn8 items or share a link to another website</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deel Learn8 items of een link naar een andere website</t>
   </si>
   <si>
     <t xml:space="preserve">Sharing_Info</t>
   </si>
   <si>
-    <t xml:space="preserve">You may have created a package that is useful for others or you know about another website for sharing learn8 files. Nice!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Je hebt misschien een pakketje gemaakt dat handig is voor anderen of je kent een website waar Learn8 pakketjes worden gedeeld. Gaaf!</t>
+    <t xml:space="preserve">You may have created Learn8 items that others may like or you know about another website for sharing Learn8 items. Nice!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Je hebt misschien Learn8 items gemaakt die anderen ook zouden kunnen gebruiken of je kent een website waar Learn8 items worden gedeeld. Gaaf!</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Fix typos in legal note
</commit_message>
<xml_diff>
--- a/docs/invariant/translations.xlsx
+++ b/docs/invariant/translations.xlsx
@@ -144,7 +144,7 @@
   <si>
     <t xml:space="preserve">Learn8 your way does not knowingly collect any data about its users, neither for itself nor for third parties. Concrete intentions:
 - If you create an account, your data is stored only on your device - not online.
-- The app will not connect to the internet by default (but if you choose to synchronize via Dropbox for example, a connection to the internet must be made and to Dropbox will store your data).
+- The app will not connect to the internet by default (but if you choose to synchronize via Dropbox for example, a connection to the internet must be made and Dropbox will store your data).
 However:
 - Even though Learn8 your way intends to provide safe software, remember that no method of transmission over the internet, or method of electronic storage is 100% secure and reliable, and Learn8 your way cannot guarantee its absolute security. Therefore, you should never use Learn8 your way for learning things that contain sensitive data. Learn8 your way cannot be held accountable for any form of data collection, data theft, or any form of damage, etcetera, by any party.
 - Even if you choose to share your learn items via a .learn8 file, the intention of Learn8 your way is to keep you anonymous - Learn8 your way does not knowingly add data to ".learn8 files for sharing" that can be traced back to you (unless you add it yourself or your means of distribution results in traceability). Despite this intention, mistakes can be made or bad design may yield unwanted results. If you choose to use the option to share data, you acknowledge this risk and you will not hold Learn8 your way accountable for it.
@@ -156,7 +156,7 @@
 - De app zal standaard geen verbinding maken met internet (maar als je er bijvoorbeeld voor kiest om te synchroniseren via Dropbox, dan zal er verbinding met internet gemaakt moeten worden en zal er wel data door Dropbox opgeslagen worden).
 Desondanks:
 - Hoewel Learn8 your way probeert om veilige software te leveren, onthoud dat geen enkele vorm van verbinden met internet of vorm van elektronische opslag 100% veilig en betrouwbaar is, en dat dus ook Learn8 your way geen absolute veiligheid kan garanderen. Gebruik Learn8 your way daarom niet voor het leren van iets dat gevoelige informatie bevat. Learn8 your way kan niet verantwoordelijk worden gehouden voor enige vorm van dataverzameling, data diefstal, of schade in enige vorm, etcetera, door welke partij dan ook.
-- Zelfs als je ervoor kiest om je learn8 items te delen via een .learn8 file, is de intentie van Learn8 your way om jou anoniem te laten; Learn8 your way voegt geen data toe aan ".learn8 files voor delen" die kan worden herleid tot jou (tenzij je dat er zelf bewust aan toevoegt of de wijze van distributie voor traceerbaarheid zorgt). Ondanks deze intentie kunnen fouten of slecht ontwerp resulteren in ongewenste werking; Learn8 your way kan privacy niet garanderen als je data deelt. Als je gebruikt maakt van de optie om data te delen, dan erken je het risico en zal je Learn8 your way daarvoor niet verantwoordelijk stellen.
+- Zelfs als je ervoor kiest om je learn8 items te delen via een .learn8 file, is de intentie van Learn8 your way om jou anoniem te laten; Learn8 your way voegt geen data toe aan ".learn8 files voor delen" die kan worden herleid tot jou (tenzij je dat er zelf bewust aan toevoegt of de wijze van distributie voor traceerbaarheid zorgt). Ondanks deze intentie kunnen fouten of slecht ontwerp resulteren in ongewenste werking; Learn8 your way kan privacy niet garanderen als je data deelt. Als je gebruik maakt van de optie om data te delen, dan erken je het risico en zal je Learn8 your way daarvoor niet verantwoordelijk stellen.
 - Hoewel Learn8 your way probeert om een stabiele leeromgeving aan te bieden met volledige achterwaartse compatibiliteit, kunnen fouten of slecht ontwerp resulteren in ongewenste werking van de app of zelfs tot bewuste wijzigingen die compatibiliteitsproblemen kunnen geven. Learn8 your way kan niet verantwoordelijk worden gehouden voor enige vorm van dataverlies, onbruikbaarheid van data of schade in enige vorm, etcetera, voor welke partij dan ook.</t>
   </si>
   <si>
@@ -2671,16 +2671,16 @@
     <t xml:space="preserve">PhyscialKeyboardQuestion</t>
   </si>
   <si>
-    <t xml:space="preserve">When using the virtual math keyboard, you can - for example - make a fraction by just typing "/" on the physical keyboard. (Note: if this setting is turned on while not having a physical keyboard attached, then two virtual keyboards might appear.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wanneer je het virtuele wiskundige toetsenbord gebruikt, kun je bijvoorbeeld via het intypen van "/" een breuk maken. (Let op: als je deze instelling aan hebt staan terwijl er geen fysiek toetsenbord is aangesloten, dan kunnen er twee virtuele toetsenborden verschijnen.)</t>
+    <t xml:space="preserve">When using the virtual math keyboard, you can still use a physical keyboard and - for example - make a fraction by just pressing "/". (Note: if this setting is turned on while not having a physical keyboard attached, then two virtual keyboards might appear.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wanneer je het virtuele wiskundige toetsenbord gebruikt, kun je nog steeds een fysiek toetsenbord gebruiken en bijvoorbeeld via het intypen van "/" een breuk maken. (Let op: als je deze instelling aan hebt staan terwijl er geen fysiek toetsenbord is aangesloten, dan kunnen er twee virtuele toetsenborden verschijnen.)</t>
   </si>
   <si>
     <t xml:space="preserve">PhyscialKeyboard_Allowed</t>
   </si>
   <si>
-    <t xml:space="preserve">When using the virtual maths keyboard, you can - for example - make a fraction by just typing "/" on the physical keyboard. (Note: if this setting is turned on while not having a physical keyboard attached, then two virtual keyboards might appear.)</t>
+    <t xml:space="preserve">When using the virtual maths keyboard, you can still use a physical keyboard and - for example - make a fraction by just pressing "/". (Note: if this setting is turned on while not having a physical keyboard attached, then two virtual keyboards might appear.)</t>
   </si>
   <si>
     <t xml:space="preserve">_LanguageResources\Tags</t>
@@ -3471,7 +3471,7 @@
   <dimension ref="A1:I363"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>